<commit_message>
added 100 cases to ai data
</commit_message>
<xml_diff>
--- a/asapData/rawData/aiGenerated.xlsx
+++ b/asapData/rawData/aiGenerated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="161">
   <si>
     <t>ai_prompt</t>
   </si>
@@ -583,6 +583,992 @@
 Overall, computers are incredible tools that provide immense opportunities for education, work, and entertainment. But just like any tool, responsible usage is essential for success. With a proper balance between technological use and regular physical and social activities, everyone can make the most of the wondrous invention that is the computer.
 Sincerely,
 [Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have had on people's lives and to persuade readers to agree.
+In the present day of innovation, computers have become an integral part of our lives. As such, computers have had a profound impact on society. In terms of the educational field, computers have enabled students of all ages to have access to unlimited amounts of information, preparing them for the active role they play in their community. In the workforce, computers are used for everything from data analysis to communication, allowing businesses to complete tasks more efficiently. 
+Apart from the obvious benefits computers bring, I urge readers to consider the potential drawbacks they also carry. In terms of the educational sector, easy access to computers has shortened everyone's attention span and some students may neglect to learn basic skills such as proper grammar and spelling. Inevitably, this could lead to a decline in actual educational performance. Additionally, in the workplace, over-reliance on computers can lead to a decrease in creativity and productivity. As a result, businesses may struggle to stay competitive and successful. 
+In conclusion, computers have brought about incredible advantages for people in educational and workplace settings. However, it is essential to be aware of the potential drawbacks and take into consideration how to best manage the use of computers in order to ensure they remain a positive influence.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+With the ever-growing presence of computers in our society, I would like to discuss their effects on the people that interact with them. In my opinion, computers have made a positive impact on the world, both through their technical capabilities and the opportunities they have created for social interaction.
+On the technical side of things, computers have allowed us to do many things that simply were not possible in the past. From the crunching of complex mathematical equations to the synthesis of complex music, computers have vastly expanded the possibilities for intellectual discovery. Not only that, but computers have allowed us to communicate with one another more quickly and efficiently than ever before. Video calls, emails, and text messages are now commonplace items of communication, and we can share information with one another without physical presence.
+But computers have also enhanced interpersonal relationships in many different ways. For example, individuals that experience difficulty in connecting with others physically have used computers to socialize and build relationships in entirely new ways. As such, computers have become a means of uniting individuals that otherwise would remain disconnected. In addition to this, computers facilitate virtual meetings and conferences, enabling people to learn cooperatively in even the most remote locations.
+In my opinion, computers have had a substantial effect on our society. Collaboration, creativity and connections are now achieved with greater efficiency and breadth than ever before. I encourage your readers to look beyond the physical aspects of computers and recognize the positive effects they have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+As a life-long consumer of technology, I would like to express my opinion on the effects computers have on people. Computers aid individuals in various tasks, but they can also serve as a distraction. 
+In recent years, computers have become an imperative tool used in the workplace and in our everyday lives. Without the use of computers, businesses could not efficiently operate, and our lives would be complicated by endless paper work and wasted time. However, computers have been found to have a detrimental impact on those who use them. 
+Time management is an area that can be greatly affected by the use of computers. Those who neglect their daily routine in favor of spending time on the computer will be unable to upkeep their other activities. This can result in a decrease in productivity and poor performance, both at work and in school. 
+Furthermore, computers can also lead to social disconnection. Unhealthy use of computers can lead to isolation, which can affect an individual's overall mental and physical health. Those who are constantly found in front of a computer screen are often disconnected from the environment around them, and they miss out on valuable social interactions. 
+Despite the negative effects of computer usage, computers can also serve as a tool to increase productivity and bring families and individuals closer together. With appropriate scheduling and interspersed computer and outdoor activity, these contraptions can serve as a means to a positive outcome in our lives.
+In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing in response to the current debate surrounding the effects of computers on people today.
+In my opinion, computers have had a tremendous and overwhelmingly positive impact on people’s lives. Firstly, computers have made communication more accessible than ever. Everyone from family members who live far away to business professionals can now connect quickly and easily due to digital tools like email, text messaging, and video messaging.
+Secondly, computers have allowed for more streamlined work processes. We can now store large quantities of data on computers, retrieve it quickly, and share it easily with others. This has allowed businesses to increase productivity, complete jobs faster, and boost overall performance.
+Finally, computers have also made learning more convenient. Through the use of online classes, students can learn the same material they would in a traditional classroom setting, but in a more flexible, affordable, and convenient way.
+Overall, computers have had a huge positive impact on people. For these reasons, I encourage readers to see and understand the many positive benefits computers have to offer.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor:
+In recent years, the introduction of computers into our everyday lives has drastically changed the way people interact with each other and the world around us. As technology continues to evolve, there should be increased focus on the potential effects computers have on people.
+Computers have revolutionized our world and made communication easier by giving individuals instant access to information–a great advantage in the moment, but can come with drawbacks. Studies have suggested that extended use of computers can lead to various physical and mental health issues, such as obesity, vision problems, and social isolation. With the prevalence of technology in our society, it is important to stay mindful of how far we let technology shape our lives.
+On the other hand, there are also many positive effects of computer usage. Computers can help to foster creativity and productivity, as well as provide a platform for communication that is not otherwise readily available. Social media platforms, for example, promote a sense of community across long distances, allowing individuals to be connected even without ever meeting in real life.
+It is important that we find a balance between too much and not enough computer usage, and this can be accomplished by maintaining a sense of awareness about the effects of computers on people. We should consider both the potential benefits and disadvantages when it comes to using technology, and implement necessary strategies to ensure that computer use is used as a tool to supplement rather than supplant our daily lives.
+Sincerely, 
+[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+In today's modern world, computers have become an essential part of everyday life. From businesses to schools, they are everywhere. Some people argue that computers bring us only positive effects, while others disagree.
+I believe computers have both positive and negative effects on people. On the positive side, computers can make life easier by allowing us access to vast resources of knowledge. Computers can also help us stay connected with family and friends in faraway locations. They can also make life more efficient, allowing us to automate tedious tasks and complete large ones quickly.
+On the negative side, too much reliance on computers can have serious implications. It can have a detrimental effect on our physical health due to lack of physical activity. Also, too much time spent in front of a screen can lead to poor mental health and take away from valuable time spent with family and friends.
+In conclusion, computers have both good and bad effects on people. We cannot ignore the fact that computers can be extremely beneficial, but we should be aware of their potentially harmful consequences. We should use them responsibly and in moderation.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to voice my opinion on the effects of computers on people's lives. As a proud member of the 21st century, I fully believe that computers have had an overwhelmingly positive effect on most aspects of our lives. 
+On the practical side, computers enable us to perform numerous everyday tasks quickly and efficiently - from online banking, to online shopping, to basic research. They also give us access to an almost limitless pool of knowledge, from which we can continue to learn and grow in almost any area. This access provides unique opportunities for people looking to start their own businesses, or for those who could use technological skills to enter a new career.
+On the societal side, computers have allowed us to connect with and understand people around the world. We are able to bridge gaps of language and culture, advancing our collective understanding of one another. Advanced technology has eradiated laborious tasks in many industries and saved countless man-hours. Significant investments in artificial intelligence and robotics have opened up the potential to introduce new and innovative ways of doing things faster, better, and with fewer resources.
+In summary, computers have infiltrated almost every aspect of our lives, for better or for worse. Many of the advances have been extremely beneficial, and I, for one, am thankful for every single one of them. 
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear [editor's name],
+As technology continues to evolve, the role of computers in our lives has become ever more significant. There are both positive and negative consequences associated with our increasing dependence on technology. My opinion is that computers have had a largely beneficial effect on people.
+For starters, the convenience that computers have provided us with is unquestionable. We’re able to communicate, find information and connect with others in moments, without having to leave the comfort of our homes. This level of efficiency and speed has allowed for numerous opportunities to arise for professionals, students and everyday citizens. 
+Furthermore, computers offer a variety of educational programs and resources that make learning more accessible. Students of all ages have been able to stay up to date with their studies and explore new intellectual territories without leaving their desks. This has allowed countless individuals to become skilled in countless fields, while also providing others with jobs that they may have otherwise struggled to obtain. 
+On top of all this, the use of computers has allowed us to save a great deal of energy and money. Thanks to virtual meeting applications, we no longer have to fret over long commutes or unnecessary travel expenditures. This means that we can complete complex tasks remotely and maintain productive relationships with other businesses and organizations. 
+At the end of the day, computers have emerged as a key component of our modern lives. They have proven to be a powerful tool capable of improving our lives in ways that prior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+Recently, there have been many changes in the world due to the impact of computers. As a result, it has been a common topic of discussion regarding the effects computers have had on people. With this in mind, I would like to take this opportunity to state my opinion on this topic.
+Personally, I believe computers have had both positive and negative effects on people. On one hand, computers have made many tasks easier and more convenient. We can now communicate with each other from any corner of the globe and accomplish a variety of tasks faster than ever before. In addition, the computer has eliminated the need for tedious and superficial paperwork, allowing us to focus on more important jobs.
+Meanwhile, computers have also had some negative effects on people. For instance, increased computer usage has been linked to a decrease in social interaction, leading to more isolated lives. Some fear that as more people rely on computers to help them with their daily tasks, they will lose the skills that come with manual labor, increasing the rate of unemployment.
+Preventing the possible negative effects of computers can be done by setting reasonable boundaries and educating the younger generations. It is important that we all take responsibility to ensure the right use of technology in our lives.
+Overall, computers have had both beneficial and harmful effects on people, which is why it is important to take the right actions and use computers responsibly. 
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor of [Newspaper Name],
+As technology continues to advance, the question of how computers affect our lives both positively and negatively is increasingly becoming relevant. Modern computers are capable of making our daily lives simpler and more productive, but there is a point at which computers can have negative effects.
+Let me start with the positives. With the advent of the internet and the ability to transfer information quickly around the globe, computers have made communication faster and more economical. By making advances in the fields of science, medicine, engineering, and education, computers are valuable assets for furthering our knowledge and helping us stay informed.
+That said, there are some potential risks as well. Spending too much time behind computer screens can lead to physical inactivity, which can increase one’s likelihood of developing health issues such as obesity and diabetes. In addition, the prevalence of computers and subsequent decrease in paper use has adversely affected our environment.
+In conclusion, while computers have been incredibly beneficial, we must always be mindful of the risks associated with their overuse. We need to take time away from screens and bring back traditional paper-based activities, while using computers in ways that are beneficial.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have had on people's lives. With the increasing presence and use of technology in our everyday lives, it is hard to ignore the effects computers have had and continue to have on the way people interact and work.
+On one hand, computers can increase productivity and offer access to an ever-growing library of knowledge. Where people might not have had easy access to information such as books, documents, and more, they now are able to find almost anything with just a few clicks on the internet. They can connect with friends and family over the internet, and look up things like recipes, literature, and news, allowing them to become more informed citizens.
+On the other hand, computers can have negative effects too. They can desensitize people from tangible interactions, leading to isolation and disconnection from physical relationships. Computers can also be detrimental to people’s health, as hours of sitting in front of a screen can cause long-term physical ailments.
+The positive and negative effects of computers must be weighed in order to make sure we can utilize its advantages without neglecting the harm it may cause. Those who use it for extended periods of time should follow safety guidelines to ensure their well being.
+In conclusion, it is essential to recognize the advantages and disadvantages of computer use, and use the technology in a healthy and reasonable manner.
+Sincerely,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing to express my opinion on the effects of computers on people. 
+In today’s world, technology is ever-evolving and more people than ever are using computers for everyday tasks. Computers have revolutionized both businesses and people’s everyday lives. Now, our access to knowledge, communication and opportunities is greater than ever.
+As computer use is on the rise, there has been increasing conversation about the risks that too much screen time may pose to people. Although it is true that too much screen time could potentially have negative effects on people, the positive effects profoundly outweigh the risks.
+The ability to connect with people around the world through online tools has exposed people to different cultures and ideas. Through computers, people can access a wealth of information and resources - far greater than what is available through print or other media sources. Computers further serve to simplify people’s lives by automating tasks which would have been laborious if done by hand.
+Of course, it is important to use technology responsibly. Sedentary lifestyle induced by excessive screen time could lead to bad health. Families should also ensure that computers are used by children safely by monitoring their online activity and the amount of time spent on the computer.
+In conclusion, the applications of computers are beneficial to people. Keeping a balance between online and offline activities is important to ensure that the use of computers will be beneficial to us all.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor,
+I am writing to express my opinion on the effects computers have had on society. Computers are one of the greatest inventions of the 20th century; they have revolutionized how we communicate, access information and operate in daily life.
+However, as technology has advanced, there are some drawbacks to using computers; they can often cause people to become disconnected from their physical environment and from one another. For instance, with the internet, there’s often less of an emphasis on face-to-face interaction. People have the potential to become so engrossed with their computers that they miss out on important experiences, like the joy of being in the presence of family and friends.
+I believe that while computers are incredibly beneficial and essential tools in this day and age, it is important to find a balance between virtual and real-life connections. We shouldn’t forget how important it is to be physically present and to interact with one another. In addition, computers have been stated to have caused stress, anxiety, and poor eating and sleeping habits. It is important for people to become aware of these potential risks and to take steps to find a healthy balance between digital and physical connections.
+In conclusion, computers can be a great asset to our lives, but we must use them responsibly and take measures to prevent them from getting in the way of our relationships with other people.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion regarding the effects computers have on people and to persuade the readers to agree with me. As technology has advanced, people of all ages have become increasingly reliant on computers. A computer can be such a helpful device, but it can also have a great impact on our physical, mental, and emotional wellbeing.
+Firstly, spending long hours sitting and using a computer can lead to physical health issues, such as back and neck pain, as well as vision problems due to straining your eyes to read the computer screen. Secondly, too much time spent on a computer can also have a negative impact on our mental health. It can lead to stress and anxiety from constantly needing to stay up-to-date with the latest news, or from making sure you don't miss out on any emails or messages. It can also cause depression, as socially connecting with people through the internet can never be a complete substitute for real-life interactions. And lastly, computers can also affect our emotional wellbeing. The feeling of loneliness that comes from sitting in front of a computer for hours can be quite overwhelming and lead to feelings of isolation. 
+In conclusion, it is important to be mindful of the effects computers have on our wellbeing and to be conscious of how much time we spend using them. Balance is key here, and makes the world of a difference in terms of wellbeing. 
+Thank you for your time and consideration.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor, 
+For years, we’ve been told that computers are revolutionizing our world and changing the way we think, work, and communicate. Now more than ever, people rely on computers to navigate their lives, but sometimes their impact is not all positive. 
+Recent studies have suggested that extensive computer use can actually have negative effects on people. Over-exposure can lead to a decrease in physical activity, poor posture, and more sedentary lifestyle. In addition, spending too much time using a computer can cause eye and wrist strain, as well as an increase in tension and stress levels. Over time, this could lead to more serious mental health issues and even serious physical conditions.
+Furthermore, addiction to computer games and access to inappropriate content on the internet could take a toll on our children. If a parent or teacher does not monitor their exposure to these types of contents, the online environment can become very dangerous.
+We must recognize the long-term risks and be aware of how we use computers. We must limit our exposure and understand that not all computer uses are beneficial. Our goal must be to ensure that computers are a positive tool that leaves no negative impacts on our lives. 
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+As our world continues to become more technology-driven, many of us are struggling to find a balance between the benefits of computers and the potential negative side effects. From my personal experience, I believe that computers have had a profoundly positive effect on our lives. 
+The most obvious benefit of computers is access to information. With a few clicks on a keyboard, we now have the ability to look up almost any subject imaginable. Computers have also improved our ability to communicate with others. Through email, video calls and chat options, we can stay connected with our friends and family around the world. 
+But the advantages of computers don’t stop there. Access to computers has made it easier for us to access educational opportunities, enabling us to gain new skills and knowledge without switching on our TVs or opening a book. They have also made it easier for us to pursue our interests and hobbies, from playing educational games to using social media sites. 
+I believe that computers can have a positive effect on people, if they are used responsibly. By limiting the amount of time we spend on our devices and accessing age-appropriate content, we can take advantage of all that computers have to offer without succumbing to their potential drawbacks. 
+Thank you for taking the time to consider my opinion on this matter. 
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing in to share my opinion on the effects computers have on people and to persuade others to agree with me.
+In recent years, technology has drastically improved the lives of many. Computers allow people to stay in touch more easily, work more efficiently and access more information than ever before. With the internet, you can now travel the globe from the comfort of your own home and access knowledge from any place in the world. 
+The effects of computers on people, however, may be both positive and negative. On the one hand, people are able to stay in constant communication with their friends and loved ones, and the internet makes it easier to access the news and keep up with the rest of the world in ways not previously possible. On the other hand, it can be argued that people become more and more isolated and detached from the world around them as they dive deeper into their computers. We are no longer engaging with the people around us and instead engaging with the digital world which can have negative impacts on our mental health. 
+Overall, computers provide wonderful advantages to our lives and I believe that the key to utilizing them in a healthy way is to balance our time spent in the digital world and the time spent being present in our real world. 
+Sincerely,
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+Dear [Editor],
+I am writing in response to the current debate around the impacts of computers and technology on people in [your community]. As a member of the community, I want to voice my opinion in this matter. 
+As a society, we have seen great advancements and efficiency because of the effects of computers and technology. Businesses have become more efficient, communication has become more instantaneous, and services have become more readily available. Everything that we do today is, in some way, made possible by computers or technology. 
+However, I worry about the range and scale of the effects of computers and technology. Young people today spend hours of their day connected to technology, leaving little room for outdoor activity, interpersonal relationships and creativity. Social media can become a source of anxiety, and the world of gaming can lead to decreased social and physical activity. 
+Although computer and technology have been beneficial, I believe we should take more steps to limit their influence. Schools should prioritize time outdoors and digital minimalism as part of teaching. Parents should also ensure that their children are not over-consuming technology, setting boundaries, and utilizing unplugged time. 
+In conclusion, I believe computers and technology have amazing potential, but it’s important to be mindful of their impacts on society and the people in it. Putting safeguards and limits in place, while making the most of their capabilities is key. 
+Thank you for the opportunity to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+As the use of computers has become more and more commonplace in our lives, the effects of these devices on people have become an issue of major importance. From children to seniors, computers have impacted the way we think and how we interact with others. 
+On the positive side, computers have helped to bridge socioeconomic and educational gaps among people. They have provided access to knowledge and learning opportunities for a wide range of people that would have been difficult or impossible in the pre-computer world.
+At the same time, computers have had some undesirable effects on the way people interact with each other. Excessive computer usage can isolate individuals, leading to more time alone in front of a screen instead of interacting with real people. This can have a negative effect on social activities. 
+In addition, computer usage can affect people’s attention spans, with scrolling endlessly through websites, emails and social media making it difficult to concentrate on work or other important tasks.
+While there is no denying that computers have reshaped our lives and society, we must be aware of the effects these devices can have on people. We must balance the benefits of technology with the potential drawbacks in order to maintain a healthy balance between the two.
+Thank you for giving me the opportunity to share my thoughts.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor:
+The impact that computers have had on modern life is undeniable. From work to leisure and entertainment, having access to powerful computing platforms has changed the way we live our lives and the way businesses function.
+As beneficial as computers are, their use does come with inherent risks and drawbacks. For example, research has shown that increased screen time can cause vision issues, physical pains, and even obesity. It has also been linked to increased stress levels, mental health issues, and addiction.
+The most concerning issue, however, is that of privacy. As computing technologies grow in power and ubiquity, so too do the risks of data breaches, identity theft, and other disturbing violations of privacy. As more of our lives become digitalized, our intimate data is at greater risk of falling into the wrong hands.
+For all of these reasons, I urge readers to take a more active role in managing technology use and protecting their data. Make sure that all of your devices feature the latest security protocols, limit screen time for yourself and children, and make it a point to know how your data is being used.
+I believe that if we can adopt better habits and increase awareness of the potential risks of computer usage, then we can ensure that the benefits of computing technology continue to outweigh the potential costs.
+Sincerely,
+[Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have on people’s lives and to persuade your readers that computers can be beneficial or detrimental, depending on how they are used.
+The evolution of the computer has undoubtedly brought significant advancement in many areas. Computers have enhanced communication, e-commerce, and business processes. They have enabled global reaches for knowledge and news, as well as facilitating countless other activities.
+At the same time, an over-reliance on computers can lead to a disconnect from real-life experiences. Too much time spent playing on a computer game or online can lead to a virtual life of its own, becoming the only focus of existence. Another novel concern is the danger posed by cyber-attacks which put our personal information and data at risk.
+In conclusion, computers have dramatically improved our lives, but we should use them responsibly. There are both positive and negative effects of computers, but by using computers with awareness, we can achieve a better balance.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion about the effects of computers on people. As we know, computers are an essential part of our lives today, and they have a profound effect on how we interact with the world around us.
+On the one hand, computers can be very useful and convenient, allowing us to access information, communicate quickly and efficiently, work productively, and create digital art and stories. We can even use computers to make our lives easier by automating tasks and saving us time and effort.
+But on the other hand, we are spending more and more time interacting with our computers and less with people. We are losing out on important social connections, leading to feelings of depression and isolation. We also tend to be more passive in our approach to learning and analyzing information due to the ease of locating answers on the internet.
+My opinion is that computers can both help and hinder our progress, depending on how we use them. We must make sure to not rely too much on our computers, and to also take the time to carve out personal connections with the people in our lives.
+Thank you for your time and consideration. I believe readers would find this issue interesting, and urge them to use their computers responsibly.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects of computers on people. At first, computers may seem to be beneficial in our daily lives, but I strongly believe that in the long run, it has a detrimental effect on us.
+For starters, computers have had a destructive effect on our physical health due to the sedentary lifestyle it promotes. With computers, people have less motivation to move around as everything is done on the computer. This leads to various health issues such as obesity, joint and muscle pain, as well as vision problems. Furthermore, computers deprive us from engaging in a lot of activities that developed over centuries to meet both practical and social needs.
+Another troubling effect of computers is their significant impact on our mental health. People spend extended hours using computers and spend less time chatting with their family, friends and co-workers. This results in the exclusion of real human connections and leads to feelings of loneliness and depression. In addition, computers can lead to cyber addiction which is characterized by excessive use of the computer resulting in poor work or school performance, sleep deprivation and in some cases, even anxiety and depression.
+All in all, computers have caused many social and physical problems among people of all ages. As such, I urge people to be mindful of the amount of time they spend on computers and emphasize the value of real human connections.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor:
+As our society progresses, the presence and widespread usage of computers has become increasingly prevalent. While they offer incredible convenience, they also present us with a number of challenges such as addiction, interruptions in personal relationships, and declines in job satisfaction. 
+I believe computers can be detrimental to people's mental health and well-being. In addition to the many physical effects of prolonged sitting and staring at a computer screen, computer usage can lead to a decrease in real-world interactions. People are often unable to enjoy activities and conversations outside of the home, and can begin to feel isolated and lonely. Screen time can easily become addictive, taking priority over time for physical activity, community service and face-to-face encounters.
+Furthermore, computers can be a great distraction from the job at hand. While they may provide a pleasant or stimulating distraction, they can also prevent employees from completing tasks in a timely manner and even affect their job performance. A workplace that heavily relies on computers can lead to a decline in job satisfaction, as employees may be trapped in front of a computer all day without a chance to socialize with their coworkers.
+In town, computers are everywhere and increasingly used in most occupations. For these reasons, it is important for us to remember the potential drawbacks of computer usage, and to strive for balance between technology and real-world interaction. 
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+In the digital age, computers are playing an increasingly large role in our daily lives. From work to home and everywhere in between, computers are being used to help make all kinds of tasks simpler and easier. While these advances undeniably offer a range of powerful benefits, I believe that computers can have some unintended negative effects on people.
+Firstly, I believe that computers can reduce human interaction. People are more predisposed to sending messages online rather than talking face-to-face, and contact with physical reality can be reduced as a result. Moreover, an over-reliance on computers can be damaging to our physical health. In the place of physical activity, people can be tempted to remain sedentary in front of their computer, leading to obesity and other health concerns.
+Most worryingly, I think computers can cause addiction. People can become obsessed with games or activities online and this can have a damaging effect on everyday life. In extreme cases, it can lead to social isolation and further psychological issues.
+The above is why I think people should be aware of the potential downsides of computers, and should be cautious of the amount of time they spend interacting with them. It is only through this awareness and moderation of our computer habits that we can ensure that computers remain a tool that helps improve our lives, and not a detriment to them.
+I hope that this letter has persuaded you to agree with me.
+Yours faithfully,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my views on the effects computers have on people. As part of the new generations, I can confidently state that technology has been beneficial for a lot of people and for good reasons.
+With the widespread usage of computers, many activities previously done manually have become automated. This helps save time and effort, granting us the chance to spend our valuable time on things that really matter. Moreover, it earns us the opportunity to access any information we need in almost any field we can imagine. In addition, the more we use computers, the more we sharpen our problem-solving skills, which can only be satisfied with technical devices such as computers.
+But with this new technology, there are also a few drawbacks that should not be neglected. For example, too much exposure to computer screens can lead to eye strain, headaches, or other physical health issues. Extended use of computers can also put our minds on hold, lessen communication skills, and result in social isolation as people are more inclined to stay home than going out and meeting friends.
+To make sure we make the most of this new frontier and stay safe at the same time, I suggest a healthy balance between making use of computers and staying away from them, whenever possible.
+Sincerely,
+[Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing this letter in regards to the increasing effects of computers on the current society. Computers have the potential to be both detrimental and beneficial to humanity. On one hand, computers can be used to improve the way we interact and do business. For instance, computers have improved communication within businesses and collaborate research projects for educational purposes. They can also increase productivity. 
+On the other hand, we must also consider the health repercussions of its widespread use. People who spend extended periods of time in front of a computer are more prone to obesity and muscular health issues. Furthermore, the time we spend on a computer can make us increasingly isolated in society, which can lead to further complications. 
+In conclusion, the influence of computers should be thoroughly analyzed before endorsing them as a beneficial tool. Although computers can be helpful to certain extents in certain fields, the potential dangers should be carefully weighed. We must ensure that computers do not become detrimental to our physical and emotional health. 
+I’m hopeful that by understanding the potential negative impacts, we can make a conscious effort to minimize the overall effects on society.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor: 
+I am writing this letter to share my opinion on the effects computers have on people. I strongly believe that computers have had both positive and negative influence on our lives. 
+On the positive side, computers have made tasks easier and faster. For instance, it takes one second to search for information on a computer, whereas it would have taken days to locate and research the same data before. Similarly, computers have simplified studying. For example, a student can now go online and access information about any subject in seconds, which would have been a painstaking process earlier. This has made it easier for students to stay on top of their studies and learn more effectively. 
+On the other hand, there are some drawbacks to relying on computers. For instance, people may become socially disconnected or experience physical discomforts due to long hours spent staring at a screen. Additionally, distracted multitasking is another issue that is common with computer use. Moreover, increased dependency on computers could lead to a feeling of helplessness when computer systems malfunction or crash. 
+In conclusion, computers have undoubtedly made tasks easier and faster, but it is essential to also be mindful of their potential to cause physical and psychological harm. 
+Sincerely, 
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+As the advancements in technology continue to rapidly evolve, computers have become an integral part of modern life for many people. As technology progresses, it has affected the way we interact, conduct business, receive information, and even the way we think.
+While computers have allowed us to accomplish more in a fraction of the time it used to take us, as with any tool, there are also potential downside effects. One of the biggest detrimental effects is the potential for computer dependency. When someone becomes too dependent on computers, he or she can start to feel overwhelmed and frustrated when unable to use them. This can lead to feelings of disconnection and isolation from the world.
+Another downside to increased computer usage is the potential negative effect on mental wellbeing. Exposure to too much blue light and long hours sitting at the computer can be linked to stress, anxiety and even depression. Not to mention that the dopamine rush that some experience can lead to an addiction to video games, Internet, and other technology-based activities.
+The key to avoiding this pitfalls is to use technology or computers in moderation. While computers can definitely be fantastic, powerful tools, they can also be detrimental to our wellbeing if used excessively. We need to be mindful and take regular breaks while in front of our screens.
+Sincerely,
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+Computers have had a tremendous impact on the world since they were first invented. Today, they play a vital role in our lives, from providing us with entertainment, to helping us stay connected with friends and family. However, there has been much debate about the effects computers have on people.
+In my opinion, computers can be used for both good and bad. For example, they can be a great tool for completing school work, researching information and communicating with those around us. They can also create opportunities for jobs that weren't available before. On the other hand, certain aspects of computers, such as online gaming, social media and online shopping, can be detrimental. They can lead to excessive screen time, distractions that can take away from important activities, and poor physical and mental health. 
+It's true that computers can be great for productivity, but they should also be used with caution. I believe that it's important to make sure that we don't get too caught up in technology and use it in moderation. It's important to recognize the potential harms that technology can bring and make sure that we are mindful of our time and the effects technology has on our lives.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to voice my opinion on the effects of computers on people. In today's technological world, computers seem to be a necessary part of life. We use them for work, school, communication and entertainment. But with such wide-reaching access to information comes potential danger.
+It is important to note that computers can have both negative and positive effects on people. For example, with the use of computers, we can now connect with people all over the world, access a variety of information at the click of a button, and conduct business in a fraction of the time it used to take. But on the other hand, there is evidence to suggest that increased computer use is associated with a decrease in physical activity, increased sedentary behaviour, and higher levels of stress. These problems can lead to physical and mental health problems, including obesity, depression, and social isolation.
+That being said, I believe that the advantages of using computers far outweigh the disadvantages. I think it is important that we use computers responsibly, limiting our time on them with time-management tools and tools to limit access to inappropriate content. We should also make sure our children are aware of the risks associated with computer use, and that they are learning in a safe and productive environment.
+Ultimately, I urge everyone to weigh the pros and cons of computer use and be aware that the effects can be both positive and negative. I believe if we take the time to establish healthy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor, 
+I am writing to share my opinion on the effects of computers on people. Computers are an essential part of our day-to-day lives, and they have undoubtedly come to shape our society and culture.
+At first glance, computers appear to be beneficial to our lives in many ways. We now have access to an unimaginable array of information, and computers greatly simplify many tasks and processes. 
+However, I believe that these advantages come with many drawbacks that should not be overlooked. We are now constantly inundated with an immense online presence that can be distracting, overwhelming, and even hazardous. Computers can replace physical activities, reducing our overall physical health. Additionally, they can quickly lead to an addiction to certain activities, making it difficult to maintain balance in our lives.
+It is important that we recognize the potential harms that come with computer usage, or we could find ourselves facing serious health and social problems. In order to protect ourselves and our communities, we need to be aware of how computers can take over our lives and make sure to take steps to keep a healthy relationship with them. 
+For the sake of our society and our own wellbeing, I urge you and your readers to remain mindful of the realities of computers. 
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+As computers become more and more commonplace in everyday life, I believe it is essential to take a look at the potential effects computers have on our lives. 
+It is undeniable that computers can be a great benefit. Access to information and the ability to communicate on a global scale are but two of the advantages. What's more, computers can provide an excellent workspace; some of the most difficult business problems can be solved with the help of a computer.
+However, it is also important to note that computers can also have a negative impact on our lives. So many people are now "plugged in" to their computers, neglecting personal relationships and their own physical health. Recent studies have suggested that computer use can lead to the development of unhealthy habits, including a sedentary lifestyle, poor posture, and even eye strain.
+I believe it is possible to take advantage of the benefits computers offer without sacrificing our mental and physical wellbeing. Computers can be used as a learning tool and even a device for social connection, but it must also be used in moderation. Consequently, I urge readers to be mindful of their physical, mental and emotional health; only then can we reap the potential benefits of computer technology.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+The rapid advancement of computers and their related technology has changed our world in many ways. Computers have opened up an entire universe of possibilities and connections, from the way we communicate with one another to the way we seek out information, conduct business, and even manage our personal finances. While the potential benefits of having access to technology are substantial and countless, there is cause for concern in the way computers have shaped the way that people interact and process information.
+Opponents of the technology suggest that the use of computers has reduced the amount of physical activity people partake in, as well as hindered the development of analytical skills since many users have become reliant on machines to do the thinking for them. Additionally, they argue, technology has both limits and drawbacks that can often be overlooked.
+However, I would suggest that the majority of computers can be used as a way of augmenting and supporting the cognitive abilities of mankind, rather than replacing them altogether. Organic intelligence must still be used to come to the most logical solutions, and the use of technology can be a great aid in expediting these solutions. Computers can help people think in new and creative ways, help us see past our own biases, expand our educations, and facilitate new ways of communicating with one another.
+I would urge readers to understand the benefits of computers and the ways in which they can make life simpler and more efficient. We must use computers responsibly and make sure that human thought is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+Since the introduction of computers, our lives have been forever changed. While many people consider computers as primarily beneficial, I have to disagree. While computers have certainly helped improve our lives in some regards, the effects of computers are not all positive.
+Technology can be isolating. People are constantly held hostage by screens and devices, becoming more and more disconnected from one another on a personal level. We far too often find ourselves sitting in front of the computer instead of going outside and engaging in physical activity or diversions with others.
+Moreover, computers have made it easier for people to have access to harmful, explicit content. This content not only harms children, but also gives the wrong impression about the values of the society. Computers have made it easier for these contents to be easily obtained. As if this were not enough, adolescents and children can become cynical, disaffected or violent as a result of these influences.
+All in all, while computers are incredibly useful, they are also sources of potential harm. Several cautionary measures must be taken to ensure that the use of computers is kept under control, and that the society is not left with its impure side effects.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to discuss the substantial benefit that computers have provided to people in today's world. It is true that computers have become an integral part of modern life, and this is a reality that cannot be denied.
+There are many advantages that computers provide. For example, they help to simplify mundane tasks, they increase productivity, and they offer access to a wealth of information. Additionally, computers and the internet provide a convenient platform for communication, both in business and personal circles.
+Notwithstanding these benefits, there are also potential hazards associated with the use of computers. For instance, exposure to radiation from cell phones, laptops, and other electronic devices has become a matter of concern for health-conscious individuals. Moreover, there is the risk of developing an unhealthy obsession with video games and other computer-related activities, leading to a lack of social and physical activity.
+Despite these issues, I believe that the advantages that computers bring outweigh the potential risks. This is mainly because computers can enrich our lives in a myriad of ways, and provide us with greater access to communication and education. Certainly, the advantages they offer can be enjoyed when using them in moderation, and the negative effects can generally be avoided.
+In conclusion, I am confident that this entertaining and useful technology can help us move forward in our everyday lives, and with the right approach and caution, its use can become an invaluable asset to humanity.
+Sincerely,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have on people and to persuade your readers to agree with me.
+As we enter a digital age, computers are increasingly playing a larger role in our lives. But does this mean it is all for the better? On one hand, computers can offer convenience and the potential to make work faster and easier. On the other hand, computers can bring harmful health effects, particularly to those who use them frequently or for extended periods of time. Research has indicated that excessive computer use can cause physical strain, increasing the risk of developing health issues such as carpal tunnel syndrome, poor posture, vision problems, and headaches.
+We must be mindful of the critical role computers can play in our lives and realize that overuse can adversely affect our health. We must make sure to take necessary precautions, such as proper posture, regular breaks and eye exercises.
+In conclusion, computers have a variety of benefits, but they must be used carefully in order to prevent potential health risks. I urge your readers to be mindful of their computer use and take the necessary steps to protect their health.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+As the world advances technologically and the prevalence of computers continues to grow, there has been much debate about the effects of having computers in the lives of people. 
+I believe computers have made a world of positive difference. Computers have eased society’s day-to-day operations, from banking and shopping to accessing important information in a matter of seconds. The convenience they provide has allowed more people to enter the workforce and encouraged more entrepreneurs to follow their dreams. 
+Education has also been profoundly impacted by computers. Students no longer rely on textbooks and teachers, but are now able to search for material on their own and use the resources available to them through computers. Learning has become more interactive and instantly satisfying with the access of unlimited information. 
+The leisure aspect of computers has given people instant entertainment. From streaming movies and playing online games to connecting with old friends and discovering new ones, the ease of access that computers offer has brought joy and fun to the lives of users. 
+Accordingly, many people’s lives have been improved through the use of computers. In an age where many activities are accomplished with the click of a button, it is safe to say that computers have become an integral part of our lives. 
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editors,
+The world has changed drastically with the development of computers and technology. Every day, people are relying more and more on their computers for many different purposes. From students to office workers, computers have made our day-to-day lives significantly easier, more efficient, and more productive. As a result, we are witnessing the integration of computers into almost every aspect of our lives.
+However, despite their many benefits, I believe that computers are having a detrimental effect on people. More and more, people are opting to carry out their activities via computers, leading to a lack of basic human interaction. As traditional face-to-face conversations decline, people are becoming more and more isolated.
+At the same time, there is a growing reliance on computers to provide facts and knowledge, leading to a decline in critical thinking. People are relying on information that is accessible via computers instead of utilizing their own brains to think, analyze and solve problems.
+Considering all the negative effects that have arisen from our increased use of computers, I feel that it’s time that the public takes a step back and examines the role computers play in our lives. We need to limit our reliance on computers and encourage people to interact with each other in a real way.
+I implore your readers to consider the benefits of using computers responsibly and for their originally intended purpose only: to make our lives easier, not more complicated.
+Sincerely,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear [Newspaper],
+As the world continues to undergo digital transformation, more and more people are utilizing the technology of computers to pursue various means of communication, entertainment, and learning. Computers are changing the way we interact with each other and the rest of the world, creating a digital revolution that is difficult to ignore.
+In my opinion, the impact of computer technology on people is both positive and beneficial. Most obviously, the use of computers in our society streamlines the way that we work and engage with others. Computers are improving communication, providing increased accuracy and speed while drastically reducing the cost of certain tasks. Computers are not only making tasks easier; they are also opening up entirely new avenues of possibility. For instance, the use of computer technology has allowed us to share our ideas, products, and services with people around the globe. 
+Moreover, the use of computer technology has also proven to be very beneficial in terms of our health. are many medical applications of computer technology that are helping to improve our lifestyles and the way that we address medical issues. From medical software to robots and other medical advancements, computers are rapidly revolutionizing the world of healthcare.
+In conclusion, computers have a very positive and useful role in our society. The use of computer technology has drastically changed the way people work, communicate, and receive healthcare. The positive effects of computers far outweigh the potential harms and I think it's important for everyone to be aware of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor,
+As the world has become increasingly reliant on technological advances, the question of how these developments impact our daily lives has become increasingly pertinent. Specifically, in regards to computers, I believe the impact on people’s lives has been overwhelmingly positive.
+In business and education, computers have been incredibly beneficial. They have replaced time-consuming and mass-produced tasks and have enabled us to store and analyze much greater amounts of data. Computers have allowed us to increase our productivity, remain more organized, and advance our knowledge on a range of subjects.
+They’ve also enabled us to stay in touch with the world, sharing ideas, information, and more with a few clicks of a button. I’d even argue that computer technology has been a net positive in terms of international relations, bridging divides and encouraging collaboration between different cultures in a way that would have been impossible without the help of technology.
+Of course, not all of the effects computers have on people are positive, and proper moderation and use should always be encouraged. With that said, I’d ask readers to consider all of the opportunities computers have opened up, and how much more productive, knowledgeable, and connected we are because of them. Computers have had a long-reaching and amazingly positive impact on our lives, and I believe that is something that should be celebrated.
+Sincerely,
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have had on people. From anecdotal evidence, I believe that computers have a fundamentally positive impact.
+To begin, modern computers have made life easier in a variety of ways. For instance, computers have drastically reduced the time and effort it takes to perform mundane calculations, such as bank account balances, tax calculations, and even predictions of the weather. Furthermore, computers have allowed greater access to information than ever before. With a few clicks of the mouse, individuals can have access to seemingly infinite resources of knowledge.
+Additionally, computers have allowed us to bridge the gap between cultures and countries. Through video chatting, online collaboration tools, and other services, individuals from all over the world are now able to instantly connect and interact with each other. The benefits of such instant communication are numerous, from expanding our horizons to connecting with long-lost family members.
+Last, computers have helped with human creativity. Software like Adobe Photoshop, in conjunction with powerful PCs, have enabled people to manipulate, create, and post beautiful photos and videos with very minor investment of time, money, and labor. 
+Based on these observations, I am firmly of the belief that computers are and will continue to be a positive force in our lives. I hope that my fellow readers will consider the arguments provided here and come to a similar conclusion.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+Since the invention of computers, the way people interact with their environment and the world has drastically changed. I am writing to share my opinion on how computers have had both positive and negative impacts on our lives.
+On the positive side, computers have revolutionized the way people are able to access and process information. In this innovative digital age, people have access to an abundance of information right at their fingertips. Furthermore, computers have been vital to virtually every industry and revolutionized the way humans work and think. With the use of computational power, businesses and companies have been able to optimize their workflows, realize cost savings, and create more efficient processes.
+While computers bring great opportunity, they also come with their own set of problems. Too much time spent on computers has been linked to mental health issues such as depression and anxiety, as well as physical problems like obesity and heart disease. Furthermore, large-scale automation has resulted in large-scale unemployment, and this trend is only expected to worsen in the near future. Physical ailments can come from sitting and working at a computer for too long, creating stress and aches that stay with us for the rest of our lives.
+It’s clear that computers have had enormous impacts on how we live and how we interact with our environment. As computers continue to become more prevalent, it’s important for us to be conscious of how much time we spend on them, both for our mental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have on people. It is clear that computers have made our lives easier in many ways. We can communicate quickly and have access to a wealth of information. However, it should not be forgotten that there are some serious downsides to computers that may have negative effects on people.
+For example, an increase in sedentary lifestyles can lead to physical inactivity, which can contribute to obesity, heart disease and other related conditions. It is also important to remember that the computer screens themselves can be a source of eye strain, headaches and even migraines. Furthermore, the use of computers has been linked to an increase in stress, anxiety, and even depression with excessive exposure.
+In conclusion, while computers can make our lives easier in many ways, there is a need to be aware of the potential risks associated with their use. People need to take regular breaks from their computer use, and limit the amount of time they spend on their computers. It is my hope that increased awareness can help people to avoid the health risks associated with computer use.
+Sincerely,
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor:
+I am writing to voice my opinion on the effects of computers on people and to persuade readers to agree with me. 
+We have seen computers become more and more of an integral part of people’s daily lives, with access to virtually limitless amounts of information and interaction with others. While these advancements provide us with the power to learn and share information, they also possess the potential to manipulate and even limit our thinking, behavior and growth as individuals.
+We are exposed to a variety of messages, advertisements and ideas while using computers, which may have an impact on our thoughts and decisions. Computers are also capable of storing vast quantities of information, which could affect our thinking and our outlook on life. Another potential issue with computer use is that it can create a sense of detachment from society and from other people in general. Computers can be a distraction from real life, and over-usage can lead to physical and mental health problems.
+Therefore, it is important for us to be mindful of how we use computers and digital technologies and to make sure that we take the necessary measures to protect ourselves and others from the potential dangers of too much technology. We must also be diligent in monitoring our own behavior and that of our children, especially when it comes to online activities. Furthermore, we must raise awareness of the effects of too much technology and help to create a culture in which people are mindful and responsible when utilizing digital technologies.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have had on people in recent years. As a society, we have become increasingly reliant on technology, and computers in particular, to get work done efficiently and quickly. It cannot be argued that computers have many benefits, such as improving our ability to communicate, facilitating the completion of complex tasks, and providing access to a vast pool of information.
+But reliance on computers has also introduced a host of potential problems. Last year's New York Times article, "The Computerization of Everything," reported on the rise of cyber fatigue, the feeling of being overwhelmed with the abundance of technology and feeling an inability to disconnect from it. It goes on to explain that cyber fatigue has been linked to impaired mood and decreased productivity.
+It is becoming increasingly clear that we must be mindful of our use of computers and technology. While computers undoubtedly offer convenience, they can have serious implications on our mental and physical health. We must find a balance that works best for us while still protecting us from excessive strain.
+I believe that this issue deserves the attention of citizens throughout the country. It is essential that we take the necessary precautions to ensure that new technology does not overpower us, but rather improves our lives.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+As the use of computers continues to pervade our everyday lives, it is important to assess the impacts this technology has on human development. In my opinion, regular and prolonged use of computers has a range of negative consequences.
+Computer use predisposes users to physical ailments such as vision problems, neck and shoulder pain due to prolonged sitting, and increased stress levels caused by staring at a bright monitor. Mental risks include decreased social skills, attention deficit, and an increased feeling of isolation. All of these consequences can lead to overwhelming feelings of depression in younger individuals exposed to the devices in an extended duration.
+One should be particularly careful with computers used in education settings as they greatly reduce the quality of the educational process. First, the use of computers often involves deeper engagement with activities unrelated to the main lesson. This can lead to distraction and loss of focus. It also reduces the need for analytical thinking, promoting only shallow and superficial understanding. Finally, an exacerbated reliance on computers allows students to skip the traditional way of taking notes, and produces a detriment to students’ memorization skills. 
+In conclusion, it is clear that the use of computers should be managed properly. Future generations will directly bear the consequences of our technological decisions, so it is our responsibility to make sure that the potentially negative effects are reduced as much as possible.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+As technology advances, computers now play a more integral role in our daily lives, both at home and at work. With this in mind, I’d like to take a moment to discuss the impacts computers have on us as individuals and as a society.
+In today’s world, computers are the gateway to the information superhighway. We have access to an unlimited wealth of knowledge right at our fingertips, and what a powerful and empowering tool that is. Computers help us stay organized, better understand concepts and tasks, and improves communication and productivity. 
+Not only do computers enable us to access a vast library of knowledge, but it can also help us learn more efficiently. With the use of educational software, students can engage in interactive learning games and activities to strengthen their knowledge base and understanding. These technologies also assist people with physical and mental disabilities achieve more independence in their lives.
+However, there are also some drawbacks. Over-reliance on computers has resulted in an increasing dependence on these machines, which can lead to an over-saturation of information, hindering problem-solving skills. Additionally, screen time exposure in excess can have devastating effects on our bodies, including poor posture, eyestrain and headaches. 
+Undeniably, computers are invaluable tools that can benefit us in many ways. But it’s important to remember to practice moderation and utilize these machines responsibly in order to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to share my opinion on the effects computers have on people. In this era of technology and digital advancements, it is impossible to deny the fact that computers play a vital role in our lives.
+From providing entertainment to aiding in medical advancements, computers are becoming a major influence in our everyday lives. Though computers are beneficial in a variety of ways, they also have potential to have negative effects on people. 
+Computers can have serious implications on physical health. Sitting in a static position for long periods of time causes fatigue and can contribute to long-term physical ailments such as back pain, neck and shoulder tension, and repetitive stress injuries. Additionally, the effects a bright computer screen can have on the eyes can be problematic.
+Moreover, computers can also be detrimental to mental health. Studies show that computer usage can increase stress and anxiety. Constant computer use may also lead to sleep disturbances due to reduced exposure to natural light. Furthermore, social media can encourage comparison and comparison-based unhappiness.
+To help keep the negative effects of computers at bay, it is important to practice healthy habits like taking breaks and setting limits on screen time use. Additionally, it is important to use the computer for constructive tasks and practice self-care when using it.
+Thus, computers can have both positive and negative effects on people. It is important to be aware and regulate computer use in order to reduce the potential health risks.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have on people. In light of the fact that more and more of our lives become intertwined with technology, I believe it is important to consider the implications of this increasing presence and reliance.
+In my opinion, computers have both positive and negative effects on people. On the up side, computers allow us to work quickly and efficiently, communicating and collaborating with each other in ways that were never possible in the past. Furthermore, the quick processing of transactions, such as online banking, has made life easier than ever before.
+Conversely, computers, when abused, can lead to detrimental outcomes. People may become too attached to them, leading to a decrease in social interactions with the real world. The need to be constantly connected to the digital world may also lead to mental and physical health issues due to lack of exercise and an unhealthy ratio of screen time to non-screen time.
+It is essential to properly assess and regulate the use of computers to maximize their potential benefits, and at the same time, minimize their potential risks. Therefore, I urge your readers to make responsible decisions when using computers and to remember the importance of a healthy balance between the digital and physical realms of our lives.
+Sincerely,
+[Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing to state my opinion on the effects of computers on people, and I believe it is important that readers recognize the possible positive and negative impacts of using computers. 
+Advancements in technology have made computers more accessible and powerful than ever before, allowing us to achieve more and be more productive. However, we ought not underestimate the potential effects computers can have on us. Spending too much time in front of a computer or other digital device can have a damaging effect on mental and physical health, particularly in the case of developing minds and bodies. 
+With this in mind, it is essential for us to make sure we continue to maintain a balanced lifestyle. This includes limiting time spent on computers and technology and engaging in physical or social activities. At the same time, it's important to be aware of the potential benefits that computers can bring with them. The Internet offers an unparalleled array of knowledge and opportunities that had never been available to people before.
+Therefore, I believe it is important to be mindful of how much time we devote to our computers, but also to embrace the opportunities that technology can bring us. 
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+As a lifelong learner, I’m constantly on the lookout for new knowledge and experiences. Recently, I’ve come to realise that computers have had an impact on the way people learn and interact with the world around them. 
+At the very basic level, computers are an invaluable learning tool. Through programs, software and apps, people are able to access new information much faster and more efficiently than ever before. Knowing how to use computers is now essential in the job market as well. It’s a given that anyone who wants to stay competitive in the modern working environment needs to have a good computer literacy. 
+That being said, I do believe that computers can have a negative effect too. We’ve become so dependent on them, sometimes even taking them for granted, that the human touch can be lost. I think it’s important to remind ourselves of the value of direct human interaction. In a world of screens and connections, it can be difficult to find time to develop meaningful relationships with friends, family and colleagues. 
+Overall, I believe that computers have been a positive force in our world. Through them, we can learn more, work faster and connect with others in ways that weren’t even thought possible a few decades ago. But, it’s also vital to remember the importance of social interaction and to remember that human relationships are irreplaceable. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+The world has evolved to become increasingly digital. Most people spend a majority of their time on digital platforms and technology. In this new digital era, computers have become an essential part of our everyday lives. Whether we’re at school, at home, or in the office, computers are affecting us in ways we may not even realize. 
+On one hand, computers have brought immense convenience and productivity to the lives of people. It’s a great tool for students, allowing them to easily look up information from the internet, watch instructional videos, and type and print out essays. It’s also enabled people to connect with each other and find global relationships from the comfort of their own home. 
+At the same time, we cannot deny the fact that computers are also having negative consequences on society and people. With the rise of social media and the internet, people are becoming increasingly isolated, spending countless hours scrolling through feeds and living their lives through a screen. On top of this, people are losing office jobs to automation, making it harder and harder to find work. 
+We need to be reminded of the importance of digital well-being. We should try to be mindful of how prolonged computer use can potentially harm our well-being. Computer technology brings convenience and access to knowledge, but only when used in moderation and with responsibility. 
+I urge the readers to to acknowledge the impact computers have on people and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I'm writing today to express my opinion regarding the effect that computers have on people. In my opinion, computers have acquired an invaluable place in our lives.
+The use of computers for academic purposes is invaluable. Computers can help students do their research more effectively and efficiently, search for results more quickly, and even grade tests for better accuracy. Additionally, many schools now use computers to improve communication between administrators, parents, and students. The widespread adoption of computers in education has increased teacher productivity, enabled greater collaboration between students, and enabled teachers to customize the instruction to meet the learning needs of each student.
+Computers are also very important in the business world. They can help save money, by modernizing manual operations, creating efficiencies in existing processes, and allowing businesses to communicate quickly and easily with customers and suppliers. Computers are also used in creating new products and services, allowing businesses to create and release products and services faster and more efficiently than ever before.
+In my opinion, the benefits of computers far outweigh any negatives, making them an important part of our lives. They make us more efficient, better informed, and more connected in ways that can improve productivity and increase our quality of life. I believe readers of your newspaper should recognize the many positive aspects of computers, and embrace the powerful tools they provide.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to voice my opinion on the effects computers have on people. I strongly believe that computers have tremendous potential to provide us with countless opportunities, yet there are certain risks that must be considered.
+With regards to the positive effects, computers provide us with easy access to a wide range of information. We can easily look up facts, information, and learn about any topic or subject with just the click of a button. Additionally, computers offer us the opportunity to connect with people internationally, and keep in touch with our friends and family.
+That being said, there are also some potential negative effects associated with computers. For one, they lack the human interaction that is so essential to our growth. We may feel more isolated, less productive, and have a difficult time concentrating when spending large amounts of time on the computer.
+Moreover, computers can become addictive, leading to an unhealthy amount of time spent in front of them. Too much time spent on the computer can lead to poor physical and mental health, and have a detrimental effect on the individual and those close to them.
+Ultimately, computers are tools that must be used with care and respect. With the appropriate knowledge and safety measures in place, computers can be a great asset to us and help us reach our goals.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+It goes without saying that computers have had a major impact on society, and their effects on people can be seen in many areas. On the whole, I believe that computers have had significant beneficial effects on people and I urge your readers to consider this point of view.
+For starters, computers allow people to become more efficient in their work and day-to-day tasks. By eliminating the need to calculate by hand, computers have removed many of the tedious tasks that previously bogged down productivity. In addition, computers are also extremely powerful tools for information gathering, allowing people to assess and analyze vast amounts of data quickly and accurately.
+Moreover, computers have also had a positive influence on people's social lives. Through technology such as the Internet and social media, people can interact with each other from any location and instantly share information, photos and ideas with friends and family. Communication is now faster and more efficient than ever before, and this has undoubtedly helped keep people connected in ways that were not possible in the past.
+Overall, it's clear that computers have had a profound impact on people and our society. From increasing efficiency to facilitating communication, it's obvious that computers have enhanced our lives in many ways. I urge your readers to consider the overall positive effects that computers have had on people and their lives.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+It is undeniable that the impact of computers on our lives extends far beyond being able to send an email or do a shopping order at the click of a button. Indeed, these devices have enabled us to access knowledge, stay connected and build bridges beyond countries, generations and cultures – but such opportunities are rapidly diminishing their usefulness when it comes to our interpersonal relationships.
+Many of us have grown increasingly dependent on these machines, turning to our computers for entertainment and communication. Without a doubt, computers have developed us into a more efficient and ‘connected’ people, but are we really benefiting from this?
+Studies have revealed that with the increase in usage of computers, our social skills have decreased significantly. What’s more, we’ve become easily distracted and less productive as a result. This leads to lower levels of engagement in shared activities, such as conversations and outdoor activities – further leading to alienation and loneliness.
+Clearly, computers are an important, convenient and invaluable form of modernity and connectivity, but we must not forget the power of face-to-face communication. I am convinced that if used in moderation, computers can still be a powerful aid in our lives without entirely taking over. We should ensure that we take the time to invest in meaningful relationships with our friends, family and the wider community, instead of simply relying on technology to satisfy our needs.
+I am certain that the readers of this publication will agree that</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have on people. Computers are used for a wide range of tasks, both in our personal and professional lives. However, there is a great debate as to whether computers are helpful or detrimental to human health.
+As with any technology, there are both pros and cons to computers. On one hand, computers help people stay connected, work faster and more efficiently, and access lifelong learning opportunities. With the right digital tool, you can quickly get the information you need and be productive in an incredibly short amount of time. We are all beneficiaries of the technologies that are continually evolving, and they allow us to do more complex and innovative work.
+On the other hand, there are potential negative health effects associated with using computers. For example, light from computer screens may damage the eyes, and sitting in front of a computer can cause stress and tension. Prolonged computer use can even lead to pain in the wrists and neck. Information overload can lead to stress, anxiety, and other psychological issues.
+In sum, computers can both help and hinder our lives. Used properly, computers can improve life and make living safer, easier, and more efficient. Used improperly, computers can harm our health and lead to various stress-related ailments. It is up to the user to be mindful of how much computer use is too much, and to balance computer use with physical activities and social interaction.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,  
+Technology is advancing at an extraordinary rate, and with it, the prevalence of computers in our daily lives is increasing. This newfound convenience has become both a blessing and a curse to our society. While computers make everyday tasks easier, they can also have a detrimental effect on people.
+On one hand, computers provide us with an abundance of information and endless possibilities for improving our lives. They make it possible to do research and learn in ways never before imagined, providing countless opportunities for growth and development. In addition, computers can help connect us with people all over the world, enabling us to build friendships and stay in touch with loved ones.
+On the other hand, computers have the potential to harm our physical and mental health. Increased computer usage can lead to poor posture, sore eyes, and fatigue. Furthermore, excessive time spent on social media can impact our mental well-being, leading to feelings of depression, isolation, and anxiety.
+Given these effects, computer usage should be exercised with caution. Use computers to your advantage – as a tool to increase knowledge, build relationships, and make life easier. But remember to unplug occasionally and engage in activities that don’t rely on technology.
+I urge you, the readers, to remember the importance of balance when it comes to computers and to practice moderation in their use.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing in response to the increasing number of people using computers today. As a supporter of technology, I understand the great benefits computers bring to our daily lives, but I also recognize some of the negative impacts computers can have.
+First, increased usage of computers poses a danger to our health. Too much time sitting in front of a computer can cause physical exhaustion, headaches, and fatigue from staring at screens for too long. Recent studies also suggest there may a link between computer usage and development of behavioral problems such as depression, difficulty concentrating, and anxiety.
+Second, over-dependence on computers could lead to a decrease in creativity and problem-solving abilities. For instance, many students neglect to practice critical thinking skills as a result of having access to so much online information. Simply entering a query into a search engine often produces instant answers to one’s queries without any thought or effort required.
+In conclusion, while computers do make our lives easier in many ways, there is no denying that extended computer usage has a number of possible adverse consequences. It is essential to be proactive in combating these issues by using computer technology in moderation and educating people in its proper use. 
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+As technology continues to become more and more pervasive in our lives today, computers undoubtedly play a hugely influential role in our daily routines. We all know the extensive potential and benefits computers offer, from educating the next generation to advancing medical research, but it is also important to pause and consider what the effects of such a powerful tool can be on us as people. 
+Research shows that using computers, tablets and phones for extended periods of time can have significant physical and mental health repercussions, from increasing stress levels, to change in physical posture, to sleeplessness and anxiety. The reliance on computers can also have a negative social and emotional impact, as we increasingly turn to our devices instead of to friends and family. 
+All this is not to say that computers are inherently all bad. Quite the contrary, it is to move towards an appreciation for their use as an important tool, as opposed to allowing them to become our ultimate source of identity, comfort and knowledge. We must recognize our individual limits with regards to how much time and reliance we trust our machines to be our only constants.
+For these reasons, I urge you and your readers to really think about the effects of using computers on your personal health, relationships, and overall well-being. Computers can be incredibly beneficial if used responsibly and with mindful awareness of their potential for danger. 
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor:
+As our world continues to evolve and develop, society is becoming increasingly reliant on computers. Over the last decade, computers have become a necessity in nearly every aspect of our lives—from purchasing groceries to completing homework assignments. While this technology is undoubtedly beneficial, it has had an immense impact on people and the way they interact with one another. 
+The primary issue with the growing prevalence of computers is that they are a form of mental distraction. As individuals of the 21st century continue to become more dependent computer technology, interpersonal relationships are suffering. Instead of communicating with individuals face to face, many people prefer to communicate over the internet. This has resulted in people developing a less strong sense of human interaction and connection. 
+The overuse of computers has also led to more sedentary lifestyles, with individuals primarily relying on technology to become informed and entertained. This, in turn, has led to an increase in obesity and longterm health issues; computer users tend to move their bodies less and tend to eat more junk food. 
+Finally, with the increased use of technology, those who do not have access to computers are becoming increasingly disadvantaged. This is mainly an issue in low-income communities and countries, where individuals are unable to access computer technology necessary to stay informed and to progress within the workforce.
+In sum, we must address the consequences that computers have had on the lives of individuals. In our increasingly digital world, computers can lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing to express my opinion on the effects of computers on people. A few decades ago, computers were not commonplace. But now, computers are everywhere. They play a major role in everyday life and have considerable effects on people.
+I am of the opinion that computers have had largely positive effects on people. Computers have democratized access to a wealth of information. From educational course materials to health advice to news, people can search and access vast amounts of information with the click of a mouse. Additionally, computers have powered advances in many industries, such as healthcare, manufacturing, and banking. From robots that assist surgeons to automated teller machines, computers have made the job easier and more efficient.
+In terms of communication, computers have improved the speed and quality of communication. Text messages, emails, and video calls make it easy to connect with friends and family. We are no longer limited by geographical distance.
+Finally, computers have allowed people to pursue creative activities, from music to art to writing. Computers and software have opened up possibilities that never existed before.
+In conclusion, computers have had mostly positive effects on people. I encourage readers to agree with me and to take advantage of the abundance of resources available to them.
+Sincerely, 
+[Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+The remarkable impact of computer technology on our everyday lives is undeniable. Computers have revolutionized how we work, how we connect with each other, and how we access information. But its effects on people can be both positive and negative, and it is important for us to recognize both. 
+On the positive side, computers allow us to do things that were once impossible. No longer do we have to manually carry out tedious calculations or organize large amounts of information. Now, with a few clicks of a button, we can instantly complete practically any task quickly and accurately. 
+Additionally, computers have enabled us to have better connections without needing to be physically close to each other. People can now collaborate via chatrooms and video-conferencing, allowing us to work together regardless of distance. We have access to the entire Web and can communicate with anyone across the globe. 
+Yet there are also some drawbacks that arise with such easy access to information and communication. People have become too reliant on computers, leading to decreased creativity and cognitive flexibility. In addition, personal information can be stolen through malicious software and malware, giving hackers access to sensitive data. Computers can also cause social isolation, as people become more and more reluctant to interact with others face-to-face.
+For these reasons, I urge readers to be mindful of the positive and negative effects of computer technology. It is a potent tool but its use should be regulated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to share my opinion about the effects computers have had on people. Over the past few decades, computers have become commonplace in everyday life, and this has had both positive and negative effects.
+On the plus side, computers have become much more powerful, compact, and integrated into everyday life. They can help us to quickly learn new skills, access information, and perform complex tasks with unprecedented speed. For example, recent advances in artificial intelligence (AI) have even enabled computers to simulate facial recognition, voice recognition, and other processes that used to require a human being.
+However, some of the effects of computer technology on people can be more detrimental. For instance, computer-based jobs can lead to social isolation and contribute to a lack of real interpersonal interaction. And, with the advent of AI, computers are now beginning to displace some lower-skilled workers. This is creating potential job losses for many people.
+Ultimately, computers are here to stay and their use will continue to grow. That’s why it’s important for us to consider the potential downsides of computer technology, as well as its many advantages. We should also work to ensure that its use serves the long-term interests of people, and that it does not create unnecessary employment problems.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to share my opinion on the effects of computers on people. I believe computers have both positive and negative effects, but the positive effects on our lives far outweigh the negatives, especially in today's age.
+The most obvious and beneficial effect computers have on individuals is increased productivity and efficiency. Computers can be used to quickly and easily store and share information, organize data, and track goals and achievements. They also help to speed up the process of tackling mundane tasks, allowing people the more time to focus on creative and innovative pursuits. Furthermore, computers are an excellent resource for education at all levels, allowing access to a world of knowledge with just the click of a mouse.
+On the social side, computers serve as a platform for connecting people all over the world, allowing us to keep in touch with our distant friends and family and to meet strangers with similar interests. Access to the internet opens up possibilities for networking, collaboration, and innovation.
+While there are criticisms that computer use is causing physical and mental health issues in people, particularly in children, proper attention must be paid to the way computers are being operated and the amount of time being spent in front of them. Parents and teachers need to ensure that children are encouraged to take part in physical exercise and to take regular breaks during computer use.
+In short, I believe that computers are an incredibly powerful tool that can, and should, be used to improve our lives. With</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+The advancement in computer technology has significantly changed the lives of people everywhere. From the daily lives of us all to the workplace, computers have integrated into our lives in a major way. To be sure, this incredible technology can be powerful and useful, but I believe it has been detrimental to the general well-being of the populace in various ways.
+Most notably, the amount of time people of all ages spend on computers has skyrocketed. Everyone from children to older adults are spending too much time in front of computers, and this time is often spent on less-than-productive activities such as online gaming, web browsing, and social networking. We are increasingly reliant on this technology, and as a result, people are losing the skills that are necessary to function in the physical world and interact with others.
+Additionally, this level of reliance and lack of face-to-face contact can negatively affect people's mental and emotional states. As an example, it is common for people to get caught in an unhealthy addiction to social media and other online activities. This can lead to decreased confidence, loneliness, and depression.
+At this point, computers are here to stay, but we must be mindful of how we use them. We must consciously use technology in a way that limits our reliance, helps us to stay connected with the physical world, and promotes physical and mental well-being.
+I urge you, the readers of your newspaper, to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I believe strongly that computers have a tremendous impact on people, both in positive and negative ways. For example, computers can help us find information and communicate with people from all over the world. However, this same technology can also have an addictive quality that can have an overwhelming and isolating effect on people.
+On the positive side, computers have enabled us to become more efficient and better informed. We can look up facts and statistics about current events, connect with people from distant countries, and shop online for nearly any item we want. These advances provide us with opportunities and conveniences that were not available in the past.
+On the other hand, people can easily become too dependent on computers. As digital media continues to grow, some of us may choose to stay at home, lost in the virtual world, instead of engaging with our peers in the real world. Excessive dependence on technology can lead to a lack of social skills and a loss of the ability to think critically.
+For this reason, we should look to use technology with caution. We should strive to find balance between the virtual and real worlds, allowing technology to enable human connections, facilitate communication, and supplement our everyday lives—not to overpower it.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor:
+In recent years, computers have become an indispensable tool in life. From being able to quickly search up information to helping people in their personal or professional lives, these devices have shown to have immense potential.  While computers can be of great benefit, people need to be aware of their potential for making life more difficult for their users.
+Using computers 24/7 can affect the physical and mental health of their user.  With the easy access to information and developments in technology, people can become dependent on their machines and are at high risk of developing psychological syndromes from using them. Additionally, there’s a risk of potential eye strain, backaches and other physical discomforts from sitting in the same posture for extended periods.
+Further, the extensive use of computers can have an impact on socialising with others. Uncontrolled use of computers not only isolates us from physical interaction but also takes away valuable time that could have been devoted to interpersonal communication and other activities.
+When used in moderation, computers can positively contribute to the daily life. It’s up to the individual to ensure that the benefits of using these devices are increasing more than the risk of using them. 
+I strongly encourage you to pay attention to the effects of computers and make sure that our society is aware of their potential.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing to voice my opinion on the effect computers have had on people over the years. As technology advances, so does the dependence on computers, and this has changed the way people live and interact with each other significantly.
+On one hand, computers have made life easier for people in many regards. For example, many people can now work from home which decreases their overall cost of living and gives them more flexibility to manage their own lives. Furthermore, computers have allowed individuals to be increasingly connected with the world around them, staying updated with global news and events in an efficient way.
+On the other hand, computers have had an equally concerning effect on people's lives. The time people spend using computers and the Internet has had a detrimental effect on people's physical, and possibly mental, health. Many people are increasingly sedentary, not getting the recommended amount of physical activity and spending less time with family and friends.
+Overall, the effect computers have had on people has been a mixed bag. Though there have been some benefits, the negatives easily outweigh the positives. I believe that, in order to prevent any further harm, people must increase their awareness of the effects of computers and start placing physical and mental wellbeing above convenience. 
+Sincerely, 
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor:
+It is no secret that computers have become an integral aspect of life. They have the power to create and preserve incredible works of art, to transform the educational landscape, and to increase productivity in all manner of fields. However, while computers are undeniably powerful tools, they can also have adverse effects on people.
+Throughout the years, people of all walks of life have come to be overly dependent on computers, particularly in the workplace. Excessive computer usage can lead to more serious problems, from eyestrain, headache, backache and carpal tunnel syndrome, to more serious psychological maladies such as depression, loss of creativity and reduced social abilities. Computers can even impair people’s ability to perform basic mathematical calculations.
+Another issue is the fact that much of the content and activities found online can be detrimental, especially for children and teens. From cyberbullying to cybercrime, the internet can pose a real risk to the physical and mental well-being of our loved ones.
+More than ever, individuals need to be aware of the potential effects computers can have and take steps to limit their overuse. Parents should monitor internet usage and keep children’s exposure to objectionable content to a minimum allowing time for activities that promote physical and mental health such as sports and reading. Individuals should also take regular breaks from the computer and get fresh air and exercise; this will help reduce feelings of lethargy and lack of imagination.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to state my opinion on the effects computers have on people. With the advancement of technology, computers have become an essential part of our lives. It is undeniable that computers have made life easier for us in many ways, from helping us organize our daily routines to enabling us to do business from nearly anywhere. 
+However, these same benefits can have a negative impact on people as well. For instance, working for hours in front of a computer screen can lead to physical complications such as headaches, eyestrain, and even muscular pain. Furthermore, prolonged exposure to computer screens can cause fatigue and stress. People can also become addicted to using computer systems, and this can lead to social isolation and lack of motivation.
+I believe that we should not take the advantages of computers for granted, as we must be aware of the potential dangers that they can pose. We should set limits on the time spent in front of a computer, and strive to increase our physical activity. Finally, we should ensure that computers are used to enhance our lives, not encumber it.
+Thank you for taking the time to read my letter. I hope that you find my thoughts persuasive and believe, as I do, that computers should be used judiciously and with caution.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+As technology continues to become more and more deeply embedded in our daily lives, and individual gadgets become smaller, more powerful, and more disposable, it becomes inevitable to ask how this technology impacts our lives. As computers in particular, increasingly become part of our daily lives, I would like to draw attention to their effects on people. 
+I firmly believe that computers are, on the whole, beneficial to people. Computers have facilitated rapid access to information and knowledge. This helps people in all kinds of situations, whether it be looking up medical information, researching a topic for an essay, or buying the perfect gift.  Computers have also improved productivity in almost every field, from medicine to architecture to aeronautics engineering. 
+On a personal level, computers allow us to maintain connections with loved ones who live far away, allow us to access a wealth of art and culture, and provide us with outlets for creative expression, such as designing and coding. They even go so far as to suggest new recipes for us to try!
+At the same time, of course, computer usage should be moderated. Too much of anything is unhealthy, and although computers give us access to a seemingly endless stream of knowledge, it can be easy to get lost in a virtual world and neglect the basics of daily life, such as physical activity and healthy human relationships. 
+I hope I have convinced you of computers' potential benefits to people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I believe computers have revolutionized the way we interact and experience our daily lives. Through technology, we have gained access to nearly limitless information, which can be a great asset to further our knowledge, develop our skills, and lead happier lives.
+However, too much reliance on computers can also be harmful. Growing up with technology can lead to an overall decrease in social interaction and even a lessening of cognitive skills. Too much time spent in front of a computer or phone can lead to an increase in sedentary habits, and a decrease in physical activity. For example, when studies were done on the effects of smartphones, medical professionals found that the device had impacted people's vision, posture, and even mental health. 
+Not to mention, the vast amount of information available on the internet can carry potential security risks, involving malware, viruses, and phishing attacks. Cybercrime is a real and serious issue.
+Therefore, in order to reap the benefits of technology, it is important to develop healthy habits that balance tech use with real-world interactions, physical activity, and other activities that can keep our bodies and minds healthy.
+Sincerely, 
+[Name] 
+[City]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing to express my opinion on the effects computers have on people. There are those who argue that computers have caused a decline in our physical and emotional health. I disagree.
+Computers have been around for decades, and many of us have grown up with them as a staple of our daily lives. As technology has improved, so have the opportunities that come with computers. We have been able to stay in contact with loved ones across the globe, access the world’s knowledge and collaborate with people to create amazing projects. There’s no denying that computers have been an incredible tool for us to use.
+The real question is, how have computers changed our lives for the better or for the worse? To answer this, we must first look at the way people use computers. In general, we use computers to make our lives more efficient and easier. We can use them to find information, shop and even make reservations.
+On the other hand, computers can be a source of distraction from physical activities, such as exercise and outdoor activities, as well as a hindrance to our mental and emotional health. Excessive use of computer-based entertainment can cause people to become withdrawn, anxious, and ultimately lead to potential health problems such as depression.
+The answer to this question lies in our own ability to use computers in a responsible way. By limiting the time we spend in front of the computer, engaging in physical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to discuss the effects of computers on people and to persuade your readers to agree with me that computers have a mix of positive and negative impacts on our lives. 
+Though it may seem as though world has become overly reliant on computers, they have created many advantages and conveniences that are beneficial to humans. For example, computers have made communication easier, allowing us to communicate with others any time, any day, and from any place. They also enable us to access knowledge and store data more efficiently, allowing us to apply and utilize information quickly, accurately, and easily. Perhaps the most tremendous benefit computers provide is improved productivity within various industries. They enable us to process tasks quickly, saving a considerable amount of time and money. 
+However, it would be naive to ignore the potential risks and disadvantages that computers may bring. They are, after all, electronic devices and as such have susceptibilities to viruses, backdoors and other malicious programs that can leave us vulnerable to data leakage and security breaches. Furthermore, computer software and hardware changes rapidly and therefore requires a wealth of time and money to maintain. Finally, problems have emerged regarding the heath implications, both physical and mental, which derive from too much ‘screen time’ and the potential for unequal access to modern digital technology. 
+In conclusion, though computers present a variety of risks and challenges, I believe it is important to recognize the multitude of benefits they bring,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I write to you today to express my opinion on the effects computers have had on people in today's world. As a long-time user of technology, I'm a believer that computers have enabled mankind to reach phenomenal heights, but I'm also aware of the potential negative effects they can have on people.
+In my view, computers have been a fundamental tool in advancing humanity. Technology has transformed the way we think and act, providing us with access to information, communication, entertainment, and so much more. It's also enabled us to complete many tasks efficiently, freeing us up to spend our time more productively.
+However, I believe that computers can also have a detrimental effect on individuals if not approached in a responsible manner. We've all heard our fair share of horror stories about those addicted to the internet, video games, and social media and so on; there's no denying that these kinds of situations can become very worrying.
+That's why it's important to be conscious of our activities and create a sustainable balance to ensure we don't become victims to computer overuse. Having a good understanding of technology and the possibilities it presents us can aid us in ensuring that we don't fall into the trap.
+All in all, I believe that computers are beneficial, but that it's essential to use them responsibly. Doing so can help guarantee a positive experience with technology, and a brighter future for everyone.
+Yours sincerely</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+Dear Editor,
+As technology continues to advance, computers are becoming increasingly prevalent in our lives. Our use of computers enables us to do various tasks more quickly and efficiently, however, it is important to consider the effects that computers are having on people.
+In my opinion, computers are a mixed blessing. On one hand, computers can help us gain greater access to essential information. For example, not only can we use our computer to look up helpful instructions to accomplish a task, but we can also use it to do research for a school paper or to gather data for a work project. Computers provide convenience and a wide range of possibilities for improving our lives.
+On the other hand, too much reliance on computer technology can be a detriment to our physical and mental health. Using computers often requires us to sit in one place for hours on end, with little opportunity to move around. This can lead to physical problems such as chronic pain or eyestrain. Additionally, too much screen time can lead to mental health issues such as irritability, stress, or depression. 
+Finally, overuse of computers can lead to decreased social interactions. As adults, it can be easy to get caught up in work projects and no longer make time for friends or family. Likewise, for children, excessive computer use can lead to neglect of books, activities, and socializing with peers.
+In conclusion, computers can be helpful, but we must be mindful of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+In recent years, computers have become an integral part of our lives. Most people have replaced their typewriters with laptops and their telephones with smart phones, but at what cost?
+Since the emergence of the computer age, our attention spans have been gradually deteriorating. People are constantly checking their email, browsing the internet, and playing online games, which often leads to a decrease in productivity and an increase in stress levels. The effects are starting to be felt in our homes, schools, and workplaces.
+There is no doubt that computers are a useful tool, but the downside cannot be denied. They are contributing to our society becoming more and more disconnected from the real world. We are so enthralled by the entertainment, distraction, and convenience that computers offer that we forget to take time to simply enjoy life and appreciate the world around us.
+I urge readers to consider the consequences of computer use and to think carefully about the amount of time spent with these devices. There are alternatives to computers that allow us to focus on the present and enjoy the world around us. Let’s take the time to focus on the importance of real relationships and activities that don’t involve computers.
+Thank you for your time and consideration.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing to express my opinion on the effects computers have on people. To be sure, the advent of computers has changed our lives significantly – from changing the way we communicate and conduct business to providing an environment for learning and entertainment. 
+However, it is the responsibility of those around us to make sure we are utilizing them correctly. Excessive computer use can be detrimental to our physical and mental health. Too much screen time has been linked to fatigue, poor sleep, and headaches, among other physical effects. It can also lead to stress and depression, as well as social isolation when used to replace in-person contact.
+It is not just adults who are affected by our over-reliance on computers, but children as well. A lack of balance in face-to-face interactions, outdoor physical activity, and schoolwork has been linked to an increase in behavior problems among young people. 
+Therefore, we need to recognize the potential downside of computers and take the necessary measures to minimize their negative impact. Education and regulation must be enforced to ensure we are using computers safely, both for ourselves and for our children. 
+In conclusion, computers can both benefit and hurt us depending on how we use them. It is our responsibility to be aware of the risks associated with computers and establish healthy limits with them. 
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing to express my opinion about the effects of computers on people. In my opinion, the increasing presence of computers in our lives has had a major and largely positive impact. 
+Today, computers are used to improve almost every aspect of life. They help in the automation of tedious tasks, aid in communication between people, and provide a wealth of knowledge that was previously unavailable. Furthermore, their presence fosters creativity and learning. For instance, software for music production or graphic design enables people to create projects of a greater quality in less time than ever before. We have also seen the rise of educational apps and websites, which have brought new ways of learning to students of all ages. 
+Computers have been used to spark innovation and significantly improve efficiency in the workplace. Companies are being revolutionized by the introduction of automated systems and have seen productivity increase accordingly. In addition, computers can save on costs and optimize the use of resources. 
+Overall, computers have made our lives much easier and certainly more interesting. I believe most people would agree that, while still having problems to be addressed such as cyber threats, computers are a considerable blessing.
+Sincerely,
+[Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor:
+As a lifelong technology enthusiast, I am amazed at how much of an effect computers and other technology have had on the lives of people today. With the advances in technology, people are now able to access information much more quickly and efficiently than ever before. As technology takes on an increasingly important role in our lives, it is important to understand the effects of this powerful tool.
+The most obvious benefit of computers is the amount of information they provide us. Through computers, we can now access a large range of information in just a few clicks. This ability to quickly and easily access knowledge is invaluable as people are able to stay connected and informed.
+In addition to providing access to knowledge, computers have also changed communication making it easier for people to stay in touch with friends and family. With social media and video conferencing services, people can now maintain long distance relationships from miles away. Furthermore, this ability to connect with people from around the world has helped foster an international understanding that was not possible before.
+While computers have certainly had a positive impact on society, it is important to remember that too much reliance on technology can also be problematic. People now rely on technology for many parts of their day to day lives, which can make them less adept at problem solving and decision making. This could lead to a decline in overall productivity, a rise in computer dependency, and a lack of creativity.
+Overall, computers have had a significant impact on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the editor:
+I am writing to express my opinion on the effect computers have on people. Based on my observation, I believe that computers have a positive impact on our lives and should be embraced instead of feared.
+First and foremost, computers have improved worker efficiency and productivity. Without computers, many of the tasks we do on a daily basis would be more difficult to complete. From automating mundane processes to providing access to information, computers can help us be more productive in our tasks. In addition, computers have allowed us to communicate more effectively; they connect us to people around the world in just a few clicks.
+Another benefit of computers is their potential to enhance learning. In the classroom, computers can be used to provide a hands-on, interactive learning environment for students. With the use of the internet, information can be easily accessed and students can use the information to deepen their knowledge on a subject. Moreover, online classes are becoming more common and allow students to learn at their own pace and convenience.
+Finally, computers have enabled us to entertain ourselves in ways we never imagined. We can play video games, watch movies, connect with friends, and much more. We can also obscure the lines between reality and fantasy, fostering creativity and imagination.
+In conclusion, I believe that computers have improved our lives in many ways. We should continue to use the potential computers hold to our advantage.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear [Name of Editor],
+I am writing to express my thoughts on the effects computers have had on people over the past few decades. While I recognize that computers have made many aspects of our lives easier, I am concerned about the potential negative effects of excessive computer use.
+From my own experience as well as from stories from others, I have come to believe that computers can have a detrimental effect on people's physical, mental and even emotional health. For example, increased screen time can lead to headaches, dry eyes, and fatigue. Additionally, many of us find ourselves in an endless cycle of checking email and social media accounts, thus causing us to lose the focus needed to accomplish other tasks.
+My opinion is that while computers are an integral part of many people's lives, it is important to maintain a balance with other activities and to be aware of the potential long-term health risks associated with excessive computer use. Therefore, I urge your readers to consider and take seriously the effects computers can have on their health and well-being.
+Sincerely,
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the profound effects computers have on people.
+In today's society, computers have become an integral part of our lives. We increasingly depend on computers for daily tasks, from communication to entertainment. Computers also provide access to vast amounts of information, making learning easier and more efficient. 
+However, there is also a serious downside to computer usage. We tend to disconnect with people when we interact with computers, which can have detrimental psychological effects. Furthermore, the constant barrage of notifications and alerts can lead to distraction, anxiety and even depression. Also, the environment can suffer when computers are overused, as they require large amounts of energy and generate a lot of heat, which can be taxing on the environment.
+Nonetheless, computers can still provide a great benefit to people if properly used. People can use smart technology to improve communication and collaboration with each other, rather than disconnecting. Additionally, technologies such as virtual reality provide new opportunities for people to experience the world in an enjoyable and engaging way. 
+I urge readers to consider the potential benefits of computers, but also take the necessary steps to limit their usage and mitigate the potential negative effects.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor,
+As technology advances, computers increasingly become an essential part of life. However, the rise of computer use has also had a profound effect on people in many ways. In my opinion, computers have had both positive and negative effects on society and individuals.
+On one hand, computers have made life much easier for most people. They allow us to carry out so many tasks more quickly and effectively. Computers have allowed us to access vast amounts of information on any topic, learn new skills, and stay in touch with distant friends and family.
+However, the effects of computers go beyond convenience. Computers have also changed the way we think, interact, and express ourselves. People now rely heavily on computers to think, communicate, and even to maintain relationships. This can have serious implications on our minds and our lives.
+Personally, I feel that computers have both strengthened and weakened us as a society. We have tremendous opportunities to experience the world, but also an increased risk of being isolated and disconnected. We need to find a balance between the advantages of computer use and the disadvantages.
+Thank you for your time.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor:
+I am writing to share my opinion on the effect computers have on people. As technology advances, so has the use of computers in our day-to-day lives. Computers have become a critical part of our lives and it’s important to understand the effects they have on us.
+In many ways, computers have improved our lives. Not only can we communicate with people across the world, but they have opened up the door to new opportunities, such as online businesses and self-employment. Computers also allow us to inform ourselves and stay up to date with the world around us. We can access news and knowledge from our fingertips all from the convenience of our own homes.
+At the same time, increased use of computers can can have some adverse effects on people. The rise of social media platforms, for example, can lead to negative effects on people’s self-esteem, as the internet can be a place for trolling, cyberbullying, and comparison to others. Additionally, technology has gradually been stealing our attention from other activities that used to be a part of our lives, such as social interactions and creative hobbies.
+Overall, humans are creative thinkers who are equally capable of creating and destroying. Therefore, computers can either be a tool that can be beneficial to society, or they can be a drug that is slowly deteriorating our physical and mental health. It is up to us to choose how we use these powerful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor,
+Computers have had a profound impact on our lives in recent years. From gaming, to communicating, to managing our finances, computers have revolutionized the way we live. But, with increased reliance on computers comes the risk of reduced physical, mental, and emotional well-being.
+Recent research has shown that over-exposure to computer screens can cause physical issues such as vision loss and headaches, as well as mental and emotional imbalances such as stress, depression, and anxiety. Research has also connected computer use to decreased attention spans as well as a decreased ability to manage emotions.
+We must be aware of the potential negative impacts of liberal computer use and strive to find a balance between using computers and engaging in physical activities, reading, and spending quality time with family and friends. This is especially important for children and young adults, who will be most impacted by the current technology revolution.
+Too much time spent using computers can have detrimental effects on our physical, mental, and emotional health, so we must use them responsibly. Computer use should be limited and balanced with other activities that promote physical and mental well-being.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I'm writing to share my opinion on the effects computers have on people, and to persuade your readers of the need to be vigilant about their use and the potential risks involved.
+At its core, technology and computers are tools for furthering our potential and opening up new opportunities for us to explore. The uses can range from professional and educational to recreational and entertaining. There's no argument that this type of technology can open up new worlds of possibilities and keep us connected to our global community.
+However, when used in excess or in inappropriate contexts, computers can alienate us from our real-world communities, leaving our minds and bodies devoid of healthy exercise or interaction. For example, the majority of social media attempts to make us isolated from others, and it is often common to stay up late at night playing video games. Such activities can lead to increased stress, depression, and loss of sleep.
+Furthermore, computers can also allow us to spread misinformation and even cyberbullying, which can be psychologically and emotionally damaging.
+In my opinion, it is important to be mindful of our use of computers and technology. We need to be judicious in our use of social networks, be vigilant of the information we put out, and use our computers responsibly in order to ensure that we continue to benefit from the capabilities they provide.
+Thank you for your consideration.
+Sincerely,
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to express my opinion on the effects computers have on people. Over the past few decades, computers have become a major part of our lives. They are used in almost every area of our lives, from work, education, and entertainment, to communication and shopping.
+The level of convenience technology provides is undeniable. People can now shop, book flights, and order food from the comfort of their own homes, eliminating the need for physical trips to the store or restaurant. Technology has also connected us with friends and family that are all around the world.
+However, as with any technology, it is important to properly manage it to ensure it has a positive effect on our lives. Too much time spent looking at a screen can cause physical and mental health issues, including impaired vision, headaches, and anxiety. If a computer is relied on too much, it can also create a barrier in human interaction, which can lead to social isolation.
+I strongly believe that we must all practice moderation when it comes to technology usage, and that the benefits it provides can come with risks if not properly managed. I encourage readers to take the time to go outside, build relationships with the people around us, and talk face-to-face. This will help us stay healthy and balanced.
+Sincerely,
+[Your name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+As a lifelong user of computers, I have spent countless hours researching and debugging the effects they have on people. As a result, I feel it’s important that I express my opinion on this subject.
+It is undeniable that computers have had a positive influence in many aspects of our lives. They have enabled us to do more in less time, facilitated a faster exchange of information and are generally convenient. However, we should be aware that, just like every tool, they have their drawbacks and potential harms, especially when used excessively.
+Extensive computer use can lead to increased stress, due to the pressure to perform at a certain level, difficulty to stay focused and lack of physical activity. Not to mention that the over-exposure to blue light and radiation from the screens constitute an actual health concern.
+The developing brains of children and teens may be especially vulnerable to the negative effects of computers, as their attention span and capabilities for problem-solving may be affected by excessive usage.
+Therefore, it is indispensable that people use computers with awareness and exercise moderation when it comes to their use. Parents should be informed about the proper usages and time restrictions to guarantee a healthy and productive use of technology.
+I am confident that the readers of this newspaper will agree with me that computers have been essential in the modern world, but their use should be moderated in order to avoid any potential harms. 
+Sincerely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear [name of newspaper],
+I am writing to express my opinion on the impact computers have had on people, particularly in recent years. From my own observations, I believe computers have had a largely positive effect on our lives and our society as a whole.
+It's no secret that computers have become integral parts of our daily lives. Through the internet, they have enabled us to stay connected to each other and access a vast amount of knowledge and resources. From staying in touch with distant friends and loved ones to finding new job opportunities, the internet has opened up a world of possibilities. For students and researchers, the internet has also grown into an invaluable resource for advancing their studies and knowledge.
+Computers have also had an impact on how we work. From business and finance to science and technology, computer systems have allowed us to become more efficient and productive in our careers. We are also able to process data quicker and more accurately, which has resulted in advances in many areas.
+Finally, computers have revolutionized the way we entertain ourselves. With the advent of smart phones and gaming consoles, we are now able to do more than simply watch movies or listen to music. We can also play games, write reviews, and purchase goods from the comfort of our own homes.
+In my opinion, computers have played a large role in making our lives better and more efficient. Therefore, I urge readers to join me in recognizing the value of computers and their incredible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I'm writing today to express my opinion regarding the effects computers have on people. It is widely accepted that computers have made life easier for many people, and I believe that to be true. However, I think a lot of people are unaware of the potential for these machines to harm us more than they help us. 
+Computer technology has its advantages, but it also has its share of negatives. Research has shown that spending too much time in front of a computer can lead to a variety of health problems, including sleep deprivation, depression, poor eyesight, and chronic fatigue. This not only affects our physical health, but it can also have a detrimental impact on our emotional well-being. 
+For some, using computers has become an obsession, leading to a decrease in personal relationships and human interaction. This can lead to feelings of loneliness and isolation. Furthermore, computers can be a distraction from other tasks that we should focus on, such as completing homework and spending quality time with family. 
+In conclusion, while computers have made many tasks easier, they can also have a negative effect on our health, relationships, and productivity. For this reason, I urge everyone to take precautions and limit their computer usage to a reasonable amount. 
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+The way computers have impacted people’s lives in the past two decades is startling and undeniable. The wave of technology revolutionized the way we think, work, and interact with others. People’s access to information and ability to share it has drastically increased, and I firmly believe that the positive effects computers have had on society far outweigh the potential drawbacks.
+For one, computers have increased productivity in all sectors. By replacing tasks that used to be done manually, computers have allowed members of the workforce to handle more work in faster, more efficient manner. This has allowed businesses to expand their operations and reach new markets. In addition, the use of computers has had a positive effect on our educational system. With the emergence and development of the internet, students now have access to unprecedented amounts of information that can facilitate their studies and help them develop new skills.
+Furthermore, computers provide us with a platform for active citizen participation. Social media networks, online blogs, and digital classrooms allow individuals to connect and share their ideas with others regardless of geographic location. This has opened up opportunities for innovative projects to take shape, decreasing isolation and promoting effective collaboration.
+Overall, the influence of computers on the modern world is unparalleled and stands as a testament to how they can be used to do good. From boosting productivity to encouraging citizen participation, I urge readers to recognize the impact that technology has had on our lives and to use it to create meaningful, positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+In recent years, the rise of computers has revolutionized how we do everyday tasks. From work projects to entertainment and communication, computers seem to be everywhere, and their presence has substantially affected how people interact with the world.
+While computers undoubtedly provide a host of valuable benefits, they also have negative consequences on people’s lives. The sheer amount of time people spend in front of computers reduces the time they spend on physical activity, leading to an ever-widening epidemic of obesity. Furthermore, computers have changed our social interactions by making them less personal, leading to feelings of isolation.
+For these reasons, I believe computers should be used carefully. People must make sure to not let their computer use become obsessive and prioritize physical activity and meaningful social interactions in their lives. Moreover, employers should ensure that their employees’ working conditions are back-friendly and that they are not overworked because of extensive computer use.
+The detrimental effects of computer use on our physical, social, and mental well-being should not be underestimated. I urge you to consider these issues in order to live a healthier, more balanced life.
+Sincerely, 
+[Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+As a citizen of this community, I feel that it is important to address the effect that computers have on people's lives. It is clear that computers have become an indispensable part of our lives, and they are changing the way we communicate, organize information and even purchase products.
+The use of computers is beneficial in many aspects. For example, they allow us to stay in touch with family, friends and colleagues all around the world in real-time, which wasn't possible before. They also grant us access to a world of information, which can make us more knowledgeable and resourceful. Additionally, computers are also handy in organizing our day-to-day tasks, helping us maximize our productivity and make our work-life balance more efficient.
+However, it is also important to recognize that computers can have a negative effect on people's lives. Computers can promote isolation and addiction, as their use often replaces face-to-face interaction with people, resulting in disconnected and dissatisfied individuals. Computers can also promote the gaming industry and its sometimes damaging consequences, such as gambling and the promotion of violence.
+All in all, it is important to recognize both the advantages and disadvantages that computers can have on people's lives. The benefit of using them is undeniable, but it's also important to recognize and address their potential dangers. It is only by recognizing both the ups and the downs of this technology that we can ensure that its use is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+As a concerned citizen and long-time resident of this community, I would like to share my opinion on the effects computers have on people. I believe that computers can be a powerful tool for education, creativity, and collaboration.
+With the right guidance and precautions in place, computers can become a valuable asset. They offer unfettered access to the world’s knowledge and allow students to gain an extra edge when it comes to their studies. For entrepreneurs, computers can make starting a business easier, creating more opportunities for success. And with the internet, people can share ideas and collaborate on projects in real time, no matter where they are geographically.
+However, there are also some potential negatives. Extended time spent on the computer can lead to physical health problems such as carpal tunnel syndrome and muscular aches. It’s been suggested that too much computer time can also lead to mental health issues such as depression and anxiety. So, it is important for people to take regular breaks from the computer and maintain a healthy balance between work and leisure.
+In conclusion, I wholeheartedly believe that computers can be a great asset, but it is important that we recognize their potential risks and take the necessary precautions to protect our wellbeing and productivity.
+Sincerely,
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor,
+I am writing to share my opinion on the effects of computers on people. Since the introduction of computers, technology has continued to advance, with computers becoming increasingly essential in our lives. This technology has positively impacted all of us, from providing educational and entertainment benefits to simplifying day-to-day tasks.
+However, the increasing reliance on computers has also had a detrimental effect on people. Our over-exposure to technology is leading to an increase in cases of mental health issues and lack of physical activity. Prolonged use of computers can cause eye strain, tension headaches, and weight gain. In addition, people who spend their days looking at computer screens can become socially isolated.
+It’s important to remember that while technology is a great asset, it’s important to use it in moderation. Make sure to take regular breaks, go outside, and connect with friends. Setting limits will help you limit your dependence on computers and help protect your physical and mental wellbeing.
+I urge readers to consider the potential effects of computer use on their health and make the effort to use technology responsibly.
+Sincerely, 
+[Your Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+To the Editor: 
+As our world has become increasingly reliant on technology and computers, it is vital to consider the effects they have on people. While there are benefits to having such quick access to information, I believe computers can also have detrimental effects on our lives.
+To begin, people’s attention spans and ability to think critically have been reduced by the reliance on technology. The prevalence of quick-click internet and high-speed processors has made it easier to find immediate, surface-level answers, resulting in people not taking the time to develop thoughtful responses. Additionally, computer overuse causes physical strain, often resulting in posture issues, eye strain and other health complications. Increasing technology-dependence has also led to a decline in interpersonal relationships, as people are distracted by phones and tablets instead of enjoying the physical presence of their peers.
+Furthermore, computers have made people vulnerable to cyber-attacks, which can be incredibly damaging. As cyber criminals become more sophisticated, it is easy to become a target in the online space and there has been an increase in online fraud and identity theft.
+Despite the various disadvantages that come with our digital world, it’s important to recognize the benefits computers cannot offer. Human connection, genuine conversation and creative problem solving are best achieved without relying on technology to carry us through. I believe it is best practice to be informed of computer’s effects while still enjoying the convenience they provide. 
+I encourage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dear Editor, 
+I am writing to present my thoughts on the effects that computers have had on our lives. As we now live in the digital age, computers are a ubiquitous part of our lives. They are used for a wide array of tasks, from work to entertainment. When used properly, computers can undoubtedly be beneficial. However, I believe that if used improperly and for too long, they can have a damaging effect on our lives.
+For example, frequent computer use can lead to general fatigue, as prolonged use can severely strain the eyes. Moreover, extended exposure to the light from screens can disrupt natural sleep patterns. Additionally, excessive computer use can lead to issues such as obesity, as people sacrifice physical activity for extended periods of sedentary behavior. 
+Thus, I would strongly urge readers to monitor their computer use and to take regular breaks. Take the time to go outside and get some fresh air or demonstrate physical activity after extended periods of computer use. This is especially important for younger users. Introducing activities such as walking and sports into the lives of children could prove to be beneficial, protecting them from the potential long-term consequences of improper computer use.
+In conclusion, computers are helpful and offer a number of advantages in terms of convenience, productivity, and entertainment. However, if used improperly and for too long, the effects can be damaging. I urge readers to exercise caution when using computers and to monitor their usage.
+Sincerely,</t>
   </si>
 </sst>
 </file>
@@ -940,7 +1926,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1825,6 +2811,2190 @@
         <v>60</v>
       </c>
     </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+      <c r="D94" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+      <c r="D104" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C106" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>3</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4</v>
+      </c>
+      <c r="D107" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>3</v>
+      </c>
+      <c r="C108" t="s">
+        <v>4</v>
+      </c>
+      <c r="D108" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>3</v>
+      </c>
+      <c r="C109" t="s">
+        <v>4</v>
+      </c>
+      <c r="D109" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110" t="s">
+        <v>4</v>
+      </c>
+      <c r="D110" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>3</v>
+      </c>
+      <c r="C114" t="s">
+        <v>4</v>
+      </c>
+      <c r="D114" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" t="s">
+        <v>4</v>
+      </c>
+      <c r="D115" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>3</v>
+      </c>
+      <c r="C116" t="s">
+        <v>4</v>
+      </c>
+      <c r="D116" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>3</v>
+      </c>
+      <c r="C117" t="s">
+        <v>4</v>
+      </c>
+      <c r="D117" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>3</v>
+      </c>
+      <c r="C119" t="s">
+        <v>4</v>
+      </c>
+      <c r="D119" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" t="s">
+        <v>4</v>
+      </c>
+      <c r="D120" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" t="s">
+        <v>4</v>
+      </c>
+      <c r="D121" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>3</v>
+      </c>
+      <c r="C122" t="s">
+        <v>4</v>
+      </c>
+      <c r="D122" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C123" t="s">
+        <v>4</v>
+      </c>
+      <c r="D123" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>3</v>
+      </c>
+      <c r="C124" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125" t="s">
+        <v>4</v>
+      </c>
+      <c r="D125" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>3</v>
+      </c>
+      <c r="C126" t="s">
+        <v>4</v>
+      </c>
+      <c r="D126" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127" t="s">
+        <v>4</v>
+      </c>
+      <c r="D127" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="1">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>3</v>
+      </c>
+      <c r="C128" t="s">
+        <v>4</v>
+      </c>
+      <c r="D128" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129" t="s">
+        <v>4</v>
+      </c>
+      <c r="D129" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130" t="s">
+        <v>4</v>
+      </c>
+      <c r="D130" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>3</v>
+      </c>
+      <c r="C131" t="s">
+        <v>4</v>
+      </c>
+      <c r="D131" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>3</v>
+      </c>
+      <c r="C132" t="s">
+        <v>4</v>
+      </c>
+      <c r="D132" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133" t="s">
+        <v>4</v>
+      </c>
+      <c r="D133" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>3</v>
+      </c>
+      <c r="C134" t="s">
+        <v>4</v>
+      </c>
+      <c r="D134" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>3</v>
+      </c>
+      <c r="C135" t="s">
+        <v>4</v>
+      </c>
+      <c r="D135" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" t="s">
+        <v>4</v>
+      </c>
+      <c r="D136" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137" t="s">
+        <v>4</v>
+      </c>
+      <c r="D137" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138" t="s">
+        <v>3</v>
+      </c>
+      <c r="C138" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139" t="s">
+        <v>3</v>
+      </c>
+      <c r="C139" t="s">
+        <v>4</v>
+      </c>
+      <c r="D139" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140" t="s">
+        <v>4</v>
+      </c>
+      <c r="D140" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141" t="s">
+        <v>4</v>
+      </c>
+      <c r="D141" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="B142" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142" t="s">
+        <v>4</v>
+      </c>
+      <c r="D142" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="B143" t="s">
+        <v>3</v>
+      </c>
+      <c r="C143" t="s">
+        <v>4</v>
+      </c>
+      <c r="D143" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144" t="s">
+        <v>3</v>
+      </c>
+      <c r="C144" t="s">
+        <v>4</v>
+      </c>
+      <c r="D144" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145" t="s">
+        <v>3</v>
+      </c>
+      <c r="C145" t="s">
+        <v>4</v>
+      </c>
+      <c r="D145" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="B146" t="s">
+        <v>3</v>
+      </c>
+      <c r="C146" t="s">
+        <v>4</v>
+      </c>
+      <c r="D146" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="B147" t="s">
+        <v>3</v>
+      </c>
+      <c r="C147" t="s">
+        <v>4</v>
+      </c>
+      <c r="D147" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>3</v>
+      </c>
+      <c r="C148" t="s">
+        <v>4</v>
+      </c>
+      <c r="D148" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149" t="s">
+        <v>4</v>
+      </c>
+      <c r="D149" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150" t="s">
+        <v>3</v>
+      </c>
+      <c r="C150" t="s">
+        <v>4</v>
+      </c>
+      <c r="D150" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151" t="s">
+        <v>4</v>
+      </c>
+      <c r="D151" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" t="s">
+        <v>4</v>
+      </c>
+      <c r="D152" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="B153" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153" t="s">
+        <v>4</v>
+      </c>
+      <c r="D153" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="B154" t="s">
+        <v>3</v>
+      </c>
+      <c r="C154" t="s">
+        <v>4</v>
+      </c>
+      <c r="D154" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155" t="s">
+        <v>4</v>
+      </c>
+      <c r="D155" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" t="s">
+        <v>4</v>
+      </c>
+      <c r="D156" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157" t="s">
+        <v>4</v>
+      </c>
+      <c r="D157" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" t="s">
+        <v>4</v>
+      </c>
+      <c r="D158" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="1">
+        <v>157</v>
+      </c>
+      <c r="B159" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" t="s">
+        <v>4</v>
+      </c>
+      <c r="D159" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="1">
+        <v>158</v>
+      </c>
+      <c r="B160" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" t="s">
+        <v>4</v>
+      </c>
+      <c r="D160" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="B161" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161" t="s">
+        <v>4</v>
+      </c>
+      <c r="D161" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="B162" t="s">
+        <v>3</v>
+      </c>
+      <c r="C162" t="s">
+        <v>4</v>
+      </c>
+      <c r="D162" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="1">
+        <v>161</v>
+      </c>
+      <c r="B163" t="s">
+        <v>3</v>
+      </c>
+      <c r="C163" t="s">
+        <v>4</v>
+      </c>
+      <c r="D163" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="1">
+        <v>162</v>
+      </c>
+      <c r="B164" t="s">
+        <v>3</v>
+      </c>
+      <c r="C164" t="s">
+        <v>4</v>
+      </c>
+      <c r="D164" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="1">
+        <v>163</v>
+      </c>
+      <c r="B165" t="s">
+        <v>3</v>
+      </c>
+      <c r="C165" t="s">
+        <v>4</v>
+      </c>
+      <c r="D165" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="1">
+        <v>164</v>
+      </c>
+      <c r="B166" t="s">
+        <v>3</v>
+      </c>
+      <c r="C166" t="s">
+        <v>4</v>
+      </c>
+      <c r="D166" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="1">
+        <v>165</v>
+      </c>
+      <c r="B167" t="s">
+        <v>3</v>
+      </c>
+      <c r="C167" t="s">
+        <v>4</v>
+      </c>
+      <c r="D167" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="1">
+        <v>166</v>
+      </c>
+      <c r="B168" t="s">
+        <v>3</v>
+      </c>
+      <c r="C168" t="s">
+        <v>4</v>
+      </c>
+      <c r="D168" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="1">
+        <v>167</v>
+      </c>
+      <c r="B169" t="s">
+        <v>3</v>
+      </c>
+      <c r="C169" t="s">
+        <v>4</v>
+      </c>
+      <c r="D169" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="1">
+        <v>168</v>
+      </c>
+      <c r="B170" t="s">
+        <v>3</v>
+      </c>
+      <c r="C170" t="s">
+        <v>4</v>
+      </c>
+      <c r="D170" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="1">
+        <v>169</v>
+      </c>
+      <c r="B171" t="s">
+        <v>3</v>
+      </c>
+      <c r="C171" t="s">
+        <v>4</v>
+      </c>
+      <c r="D171" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="1">
+        <v>170</v>
+      </c>
+      <c r="B172" t="s">
+        <v>3</v>
+      </c>
+      <c r="C172" t="s">
+        <v>4</v>
+      </c>
+      <c r="D172" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="1">
+        <v>171</v>
+      </c>
+      <c r="B173" t="s">
+        <v>3</v>
+      </c>
+      <c r="C173" t="s">
+        <v>4</v>
+      </c>
+      <c r="D173" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="1">
+        <v>172</v>
+      </c>
+      <c r="B174" t="s">
+        <v>3</v>
+      </c>
+      <c r="C174" t="s">
+        <v>4</v>
+      </c>
+      <c r="D174" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="1">
+        <v>173</v>
+      </c>
+      <c r="B175" t="s">
+        <v>3</v>
+      </c>
+      <c r="C175" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="1">
+        <v>174</v>
+      </c>
+      <c r="B176" t="s">
+        <v>3</v>
+      </c>
+      <c r="C176" t="s">
+        <v>4</v>
+      </c>
+      <c r="D176" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="1">
+        <v>175</v>
+      </c>
+      <c r="B177" t="s">
+        <v>3</v>
+      </c>
+      <c r="C177" t="s">
+        <v>4</v>
+      </c>
+      <c r="D177" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="1">
+        <v>176</v>
+      </c>
+      <c r="B178" t="s">
+        <v>3</v>
+      </c>
+      <c r="C178" t="s">
+        <v>4</v>
+      </c>
+      <c r="D178" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="1">
+        <v>177</v>
+      </c>
+      <c r="B179" t="s">
+        <v>3</v>
+      </c>
+      <c r="C179" t="s">
+        <v>4</v>
+      </c>
+      <c r="D179" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="1">
+        <v>178</v>
+      </c>
+      <c r="B180" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180" t="s">
+        <v>4</v>
+      </c>
+      <c r="D180" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="1">
+        <v>179</v>
+      </c>
+      <c r="B181" t="s">
+        <v>3</v>
+      </c>
+      <c r="C181" t="s">
+        <v>4</v>
+      </c>
+      <c r="D181" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="1">
+        <v>180</v>
+      </c>
+      <c r="B182" t="s">
+        <v>3</v>
+      </c>
+      <c r="C182" t="s">
+        <v>4</v>
+      </c>
+      <c r="D182" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="1">
+        <v>181</v>
+      </c>
+      <c r="B183" t="s">
+        <v>3</v>
+      </c>
+      <c r="C183" t="s">
+        <v>4</v>
+      </c>
+      <c r="D183" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="1">
+        <v>182</v>
+      </c>
+      <c r="B184" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184" t="s">
+        <v>4</v>
+      </c>
+      <c r="D184" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="1">
+        <v>183</v>
+      </c>
+      <c r="B185" t="s">
+        <v>3</v>
+      </c>
+      <c r="C185" t="s">
+        <v>4</v>
+      </c>
+      <c r="D185" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="1">
+        <v>184</v>
+      </c>
+      <c r="B186" t="s">
+        <v>3</v>
+      </c>
+      <c r="C186" t="s">
+        <v>4</v>
+      </c>
+      <c r="D186" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="1">
+        <v>185</v>
+      </c>
+      <c r="B187" t="s">
+        <v>3</v>
+      </c>
+      <c r="C187" t="s">
+        <v>4</v>
+      </c>
+      <c r="D187" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="1">
+        <v>186</v>
+      </c>
+      <c r="B188" t="s">
+        <v>3</v>
+      </c>
+      <c r="C188" t="s">
+        <v>4</v>
+      </c>
+      <c r="D188" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="1">
+        <v>187</v>
+      </c>
+      <c r="B189" t="s">
+        <v>3</v>
+      </c>
+      <c r="C189" t="s">
+        <v>4</v>
+      </c>
+      <c r="D189" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="1">
+        <v>188</v>
+      </c>
+      <c r="B190" t="s">
+        <v>3</v>
+      </c>
+      <c r="C190" t="s">
+        <v>4</v>
+      </c>
+      <c r="D190" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="1">
+        <v>189</v>
+      </c>
+      <c r="B191" t="s">
+        <v>3</v>
+      </c>
+      <c r="C191" t="s">
+        <v>4</v>
+      </c>
+      <c r="D191" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="1">
+        <v>190</v>
+      </c>
+      <c r="B192" t="s">
+        <v>3</v>
+      </c>
+      <c r="C192" t="s">
+        <v>4</v>
+      </c>
+      <c r="D192" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="1">
+        <v>191</v>
+      </c>
+      <c r="B193" t="s">
+        <v>3</v>
+      </c>
+      <c r="C193" t="s">
+        <v>4</v>
+      </c>
+      <c r="D193" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="1">
+        <v>192</v>
+      </c>
+      <c r="B194" t="s">
+        <v>3</v>
+      </c>
+      <c r="C194" t="s">
+        <v>4</v>
+      </c>
+      <c r="D194" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="1">
+        <v>193</v>
+      </c>
+      <c r="B195" t="s">
+        <v>3</v>
+      </c>
+      <c r="C195" t="s">
+        <v>4</v>
+      </c>
+      <c r="D195" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="1">
+        <v>194</v>
+      </c>
+      <c r="B196" t="s">
+        <v>3</v>
+      </c>
+      <c r="C196" t="s">
+        <v>4</v>
+      </c>
+      <c r="D196" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="1">
+        <v>195</v>
+      </c>
+      <c r="B197" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197" t="s">
+        <v>4</v>
+      </c>
+      <c r="D197" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="1">
+        <v>196</v>
+      </c>
+      <c r="B198" t="s">
+        <v>3</v>
+      </c>
+      <c r="C198" t="s">
+        <v>4</v>
+      </c>
+      <c r="D198" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="1">
+        <v>197</v>
+      </c>
+      <c r="B199" t="s">
+        <v>3</v>
+      </c>
+      <c r="C199" t="s">
+        <v>4</v>
+      </c>
+      <c r="D199" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="1">
+        <v>198</v>
+      </c>
+      <c r="B200" t="s">
+        <v>3</v>
+      </c>
+      <c r="C200" t="s">
+        <v>4</v>
+      </c>
+      <c r="D200" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="1">
+        <v>199</v>
+      </c>
+      <c r="B201" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" t="s">
+        <v>4</v>
+      </c>
+      <c r="D201" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="1">
+        <v>200</v>
+      </c>
+      <c r="B202" t="s">
+        <v>3</v>
+      </c>
+      <c r="C202" t="s">
+        <v>4</v>
+      </c>
+      <c r="D202" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="1">
+        <v>201</v>
+      </c>
+      <c r="B203" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203" t="s">
+        <v>4</v>
+      </c>
+      <c r="D203" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="1">
+        <v>202</v>
+      </c>
+      <c r="B204" t="s">
+        <v>3</v>
+      </c>
+      <c r="C204" t="s">
+        <v>4</v>
+      </c>
+      <c r="D204" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="1">
+        <v>203</v>
+      </c>
+      <c r="B205" t="s">
+        <v>3</v>
+      </c>
+      <c r="C205" t="s">
+        <v>4</v>
+      </c>
+      <c r="D205" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="1">
+        <v>204</v>
+      </c>
+      <c r="B206" t="s">
+        <v>3</v>
+      </c>
+      <c r="C206" t="s">
+        <v>4</v>
+      </c>
+      <c r="D206" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" s="1">
+        <v>205</v>
+      </c>
+      <c r="B207" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" t="s">
+        <v>4</v>
+      </c>
+      <c r="D207" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" s="1">
+        <v>206</v>
+      </c>
+      <c r="B208" t="s">
+        <v>3</v>
+      </c>
+      <c r="C208" t="s">
+        <v>4</v>
+      </c>
+      <c r="D208" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" s="1">
+        <v>207</v>
+      </c>
+      <c r="B209" t="s">
+        <v>3</v>
+      </c>
+      <c r="C209" t="s">
+        <v>4</v>
+      </c>
+      <c r="D209" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" s="1">
+        <v>208</v>
+      </c>
+      <c r="B210" t="s">
+        <v>3</v>
+      </c>
+      <c r="C210" t="s">
+        <v>4</v>
+      </c>
+      <c r="D210" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" s="1">
+        <v>209</v>
+      </c>
+      <c r="B211" t="s">
+        <v>3</v>
+      </c>
+      <c r="C211" t="s">
+        <v>4</v>
+      </c>
+      <c r="D211" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="1">
+        <v>210</v>
+      </c>
+      <c r="B212" t="s">
+        <v>3</v>
+      </c>
+      <c r="C212" t="s">
+        <v>4</v>
+      </c>
+      <c r="D212" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="1">
+        <v>211</v>
+      </c>
+      <c r="B213" t="s">
+        <v>3</v>
+      </c>
+      <c r="C213" t="s">
+        <v>4</v>
+      </c>
+      <c r="D213" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="1">
+        <v>212</v>
+      </c>
+      <c r="B214" t="s">
+        <v>3</v>
+      </c>
+      <c r="C214" t="s">
+        <v>4</v>
+      </c>
+      <c r="D214" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="1">
+        <v>213</v>
+      </c>
+      <c r="B215" t="s">
+        <v>3</v>
+      </c>
+      <c r="C215" t="s">
+        <v>4</v>
+      </c>
+      <c r="D215" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" s="1">
+        <v>214</v>
+      </c>
+      <c r="B216" t="s">
+        <v>3</v>
+      </c>
+      <c r="C216" t="s">
+        <v>4</v>
+      </c>
+      <c r="D216" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="1">
+        <v>215</v>
+      </c>
+      <c r="B217" t="s">
+        <v>3</v>
+      </c>
+      <c r="C217" t="s">
+        <v>4</v>
+      </c>
+      <c r="D217" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="1">
+        <v>216</v>
+      </c>
+      <c r="B218" t="s">
+        <v>3</v>
+      </c>
+      <c r="C218" t="s">
+        <v>4</v>
+      </c>
+      <c r="D218" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" s="1">
+        <v>217</v>
+      </c>
+      <c r="B219" t="s">
+        <v>3</v>
+      </c>
+      <c r="C219" t="s">
+        <v>4</v>
+      </c>
+      <c r="D219" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>